<commit_message>
Actualización Excel con Firma Boleta Determinación GNA
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6BB79-F987-4CCB-AE2B-C92105779FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB87A65-E870-4984-9155-EE36894BDD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
   </bookViews>
@@ -226,8 +226,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
   <si>
     <t>Mpcsd</t>
   </si>
@@ -540,6 +562,15 @@
   </si>
   <si>
     <t>{{DistribucionGasNaturalAsociado.VolumenGnsd}}</t>
+  </si>
+  <si>
+    <t>Representante UNNA ENERGIA-PGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Representante UNNA ENERGIA-Lote IV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Representante Perupetro</t>
   </si>
 </sst>
 </file>
@@ -549,9 +580,9 @@
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-280A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -862,7 +893,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -897,7 +928,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
@@ -918,7 +949,7 @@
     <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,14 +976,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,7 +1008,7 @@
     <xf numFmtId="4" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1029,10 +1060,10 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1064,6 +1095,108 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1079,116 +1212,23 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1267,218 +1307,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>145676</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>22411</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3020786" cy="311496"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CuadroTexto 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73DA6329-9758-401C-B8B4-9E93BE690D58}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="784411" y="19307735"/>
-          <a:ext cx="3020786" cy="311496"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Representante UNNA</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> ENERGIA</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>-PGT</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3401785" cy="311496"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CuadroTexto 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CEFD900-B6CC-41C0-B804-8F57A69A59F2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4840941" y="20495559"/>
-          <a:ext cx="3401785" cy="311496"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1"/>
-            <a:t>Representante</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1" baseline="0"/>
-            <a:t> UNNA ENERGIA-Lote IV</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>358588</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>212912</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2237104" cy="311496"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CuadroTexto 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1489767E-F6A6-4DCE-95C7-6C05C75D9875}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9502588" y="20484353"/>
-          <a:ext cx="2237104" cy="311496"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1"/>
-            <a:t>Representante</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1400" b="1" baseline="0"/>
-            <a:t> Perupetro</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
@@ -1631,62 +1459,71 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>784412</xdr:colOff>
-          <xdr:row>79</xdr:row>
-          <xdr:rowOff>156882</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="1873667" cy="1243108"/>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="9" name="Imagen 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CEBAD90-7999-4B43-B282-C461CE790F7B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Firmas" spid="_x0000_s1038"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1423147" y="19218088"/>
-              <a:ext cx="1873667" cy="1243108"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:softEdge rad="31750"/>
-            </a:effectLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2011,8 +1848,8 @@
   </sheetPr>
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A57" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A59" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2033,42 +1870,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="100"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="92"/>
       <c r="D1" s="59"/>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98"/>
       <c r="I1" s="58" t="s">
         <v>74</v>
       </c>
       <c r="J1" s="58"/>
     </row>
     <row r="2" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="102"/>
-      <c r="C2" s="103"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="94"/>
       <c r="D2" s="56"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="98" t="s">
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="99"/>
+      <c r="J2" s="81"/>
       <c r="K2" s="55"/>
     </row>
     <row r="3" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="104"/>
-      <c r="C3" s="105"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
       <c r="D3" s="54"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="111"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="102"/>
       <c r="I3" s="53" t="s">
         <v>72</v>
       </c>
@@ -2144,13 +1981,13 @@
       <c r="C10" s="48"/>
     </row>
     <row r="11" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="89" t="s">
+      <c r="E11" s="83" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="27" t="s">
@@ -2162,9 +1999,9 @@
     </row>
     <row r="12" spans="2:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="47"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="91"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="84"/>
       <c r="F12" s="19" t="s">
         <v>49</v>
       </c>
@@ -2180,8 +2017,8 @@
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B13" s="47"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
       <c r="E13" s="8" t="s">
         <v>45</v>
       </c>
@@ -2268,14 +2105,14 @@
     <row r="19" spans="1:9" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="95"/>
-      <c r="E19" s="112" t="s">
+      <c r="D19" s="85"/>
+      <c r="E19" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="80" t="s">
+      <c r="F19" s="103" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="17"/>
@@ -2283,23 +2120,23 @@
       <c r="I19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="80"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="103"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="88" t="s">
+      <c r="D22" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="92" t="s">
+      <c r="E22" s="86" t="s">
         <v>33</v>
       </c>
       <c r="F22" s="27" t="s">
@@ -2310,70 +2147,70 @@
       <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="92" t="s">
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="92" t="s">
+      <c r="G23" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="92" t="s">
+      <c r="H23" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="92" t="s">
+      <c r="I23" s="86" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="87"/>
+      <c r="F24" s="87"/>
+      <c r="G24" s="87"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="93"/>
-      <c r="I26" s="93"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="93"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C28" s="88"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="94"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
       <c r="E29" s="8" t="s">
         <v>45</v>
       </c>
@@ -2464,13 +2301,13 @@
     </row>
     <row r="37" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C37" s="9"/>
-      <c r="D37" s="92" t="s">
+      <c r="D37" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="80" t="s">
+      <c r="F37" s="103" t="s">
         <v>34</v>
       </c>
       <c r="G37" s="28"/>
@@ -2479,22 +2316,22 @@
     </row>
     <row r="38" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C38" s="9"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="97"/>
-      <c r="F38" s="80"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="103"/>
       <c r="G38" s="28"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C39" s="9"/>
-      <c r="D39" s="92" t="s">
+      <c r="D39" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="96" t="s">
+      <c r="E39" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="80" t="s">
+      <c r="F39" s="103" t="s">
         <v>34</v>
       </c>
       <c r="G39" s="28"/>
@@ -2503,22 +2340,22 @@
     </row>
     <row r="40" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C40" s="9"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="80"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="103"/>
       <c r="G40" s="28"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="9"/>
-      <c r="D41" s="92" t="s">
+      <c r="D41" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="96" t="s">
+      <c r="E41" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="75" t="s">
+      <c r="F41" s="109" t="s">
         <v>34</v>
       </c>
       <c r="G41" s="28"/>
@@ -2527,21 +2364,21 @@
     </row>
     <row r="42" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C42" s="9"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="97"/>
-      <c r="F42" s="75"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="109"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
     <row r="44" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="88" t="s">
+      <c r="C44" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="88" t="s">
+      <c r="D44" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="89" t="s">
+      <c r="E44" s="83" t="s">
         <v>33</v>
       </c>
       <c r="F44" s="27" t="s">
@@ -2552,52 +2389,52 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="95" t="s">
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="105"/>
+      <c r="F45" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="95" t="s">
+      <c r="G45" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="H45" s="95" t="s">
+      <c r="H45" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="95" t="s">
+      <c r="I45" s="85" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="46" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="88"/>
-      <c r="D46" s="88"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="95"/>
-      <c r="G46" s="95"/>
-      <c r="H46" s="95"/>
-      <c r="I46" s="95"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="105"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="85"/>
     </row>
     <row r="47" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="95"/>
-      <c r="G47" s="95"/>
-      <c r="H47" s="95"/>
-      <c r="I47" s="95"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="85"/>
+      <c r="I47" s="85"/>
     </row>
     <row r="48" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="95"/>
-      <c r="I48" s="95"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
     </row>
     <row r="49" spans="3:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="C49" s="88"/>
-      <c r="D49" s="88"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
       <c r="E49" s="8" t="s">
         <v>28</v>
       </c>
@@ -2648,11 +2485,11 @@
     </row>
     <row r="52" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C52" s="9"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="87"/>
+      <c r="D52" s="116"/>
+      <c r="E52" s="116"/>
+      <c r="F52" s="116"/>
+      <c r="G52" s="116"/>
+      <c r="H52" s="116"/>
       <c r="I52" s="14"/>
     </row>
     <row r="53" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2666,13 +2503,13 @@
     <row r="54" spans="3:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="57"/>
       <c r="E54" s="63"/>
-      <c r="G54" s="76" t="s">
+      <c r="G54" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="78" t="s">
+      <c r="H54" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="I54" s="80" t="s">
+      <c r="I54" s="103" t="s">
         <v>21</v>
       </c>
       <c r="L54" s="16"/>
@@ -2680,26 +2517,26 @@
     <row r="55" spans="3:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="57"/>
       <c r="E55" s="63"/>
-      <c r="G55" s="77"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="80"/>
+      <c r="G55" s="111"/>
+      <c r="H55" s="113"/>
+      <c r="I55" s="103"/>
       <c r="L55" s="16"/>
     </row>
     <row r="56" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G56" s="81" t="s">
+      <c r="G56" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="82" t="s">
+      <c r="H56" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="I56" s="83" t="s">
+      <c r="I56" s="115" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="57" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G57" s="81"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="83"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="114"/>
+      <c r="I57" s="115"/>
     </row>
     <row r="58" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="G58" s="7"/>
@@ -2739,54 +2576,54 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="3:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="C64" s="113" t="s">
+      <c r="C64" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="113" t="s">
+      <c r="D64" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="114" t="s">
+      <c r="E64" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="F64" s="115"/>
-      <c r="G64" s="115"/>
-      <c r="H64" s="116"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="78"/>
+      <c r="H64" s="79"/>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="113"/>
-      <c r="D65" s="113"/>
-      <c r="E65" s="81" t="s">
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="81" t="s">
+      <c r="F65" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="81" t="s">
+      <c r="G65" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="81" t="s">
+      <c r="H65" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="113"/>
-      <c r="D66" s="113"/>
-      <c r="E66" s="81"/>
-      <c r="F66" s="81"/>
-      <c r="G66" s="81"/>
-      <c r="H66" s="81"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="75"/>
+      <c r="F66" s="75"/>
+      <c r="G66" s="75"/>
+      <c r="H66" s="75"/>
     </row>
     <row r="67" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C67" s="113"/>
-      <c r="D67" s="113"/>
-      <c r="E67" s="81"/>
-      <c r="F67" s="81"/>
-      <c r="G67" s="81"/>
-      <c r="H67" s="81"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="76"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
+      <c r="G67" s="75"/>
+      <c r="H67" s="75"/>
     </row>
     <row r="68" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C68" s="113"/>
-      <c r="D68" s="113"/>
+      <c r="C68" s="76"/>
+      <c r="D68" s="76"/>
       <c r="E68" s="6" t="s">
         <v>11</v>
       </c>
@@ -2829,11 +2666,11 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="86" t="s">
+      <c r="B72" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="86"/>
-      <c r="D72" s="86"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
       <c r="E72" s="5" t="s">
         <v>85</v>
       </c>
@@ -2859,11 +2696,11 @@
       <c r="H73" s="13"/>
     </row>
     <row r="74" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="86" t="s">
+      <c r="B74" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="86"/>
-      <c r="D74" s="86"/>
+      <c r="C74" s="108"/>
+      <c r="D74" s="108"/>
       <c r="E74" s="5" t="s">
         <v>88</v>
       </c>
@@ -2874,11 +2711,11 @@
       <c r="H74" s="13"/>
     </row>
     <row r="75" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="86" t="s">
+      <c r="B75" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="86"/>
-      <c r="D75" s="86"/>
+      <c r="C75" s="108"/>
+      <c r="D75" s="108"/>
       <c r="E75" s="5" t="s">
         <v>87</v>
       </c>
@@ -2889,11 +2726,11 @@
       <c r="H75" s="13"/>
     </row>
     <row r="76" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="86" t="s">
+      <c r="B76" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="86"/>
-      <c r="D76" s="86"/>
+      <c r="C76" s="108"/>
+      <c r="D76" s="108"/>
       <c r="E76" s="5" t="s">
         <v>89</v>
       </c>
@@ -2908,10 +2745,10 @@
       <c r="G77" s="12"/>
     </row>
     <row r="78" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="84" t="s">
+      <c r="C78" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="84"/>
+      <c r="D78" s="106"/>
       <c r="E78" s="64" t="s">
         <v>90</v>
       </c>
@@ -2923,10 +2760,10 @@
       <c r="I78" s="9"/>
     </row>
     <row r="79" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C79" s="85" t="s">
+      <c r="C79" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="D79" s="85"/>
+      <c r="D79" s="107"/>
       <c r="E79" s="65" t="s">
         <v>91</v>
       </c>
@@ -2947,8 +2784,10 @@
       <c r="I80" s="9"/>
     </row>
     <row r="81" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C81" s="74"/>
-      <c r="D81" s="74"/>
+      <c r="C81" s="107" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D81" s="107"/>
       <c r="E81" s="65"/>
       <c r="F81" s="2"/>
       <c r="G81" s="9"/>
@@ -2956,8 +2795,8 @@
       <c r="I81" s="9"/>
     </row>
     <row r="82" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C82" s="74"/>
-      <c r="D82" s="74"/>
+      <c r="C82" s="107"/>
+      <c r="D82" s="107"/>
       <c r="E82" s="65"/>
       <c r="F82" s="2"/>
       <c r="G82" s="9"/>
@@ -2965,8 +2804,8 @@
       <c r="I82" s="9"/>
     </row>
     <row r="83" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C83" s="74"/>
-      <c r="D83" s="74"/>
+      <c r="C83" s="107"/>
+      <c r="D83" s="107"/>
       <c r="E83" s="65"/>
       <c r="F83" s="2"/>
       <c r="G83" s="9"/>
@@ -2974,8 +2813,8 @@
       <c r="I83" s="9"/>
     </row>
     <row r="84" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C84" s="74"/>
-      <c r="D84" s="74"/>
+      <c r="C84" s="107"/>
+      <c r="D84" s="107"/>
       <c r="E84" s="65"/>
       <c r="F84" s="2"/>
       <c r="G84" s="9"/>
@@ -2983,8 +2822,8 @@
       <c r="I84" s="9"/>
     </row>
     <row r="85" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C85" s="74"/>
-      <c r="D85" s="74"/>
+      <c r="C85" s="107"/>
+      <c r="D85" s="107"/>
       <c r="E85" s="65"/>
       <c r="F85" s="2"/>
       <c r="G85" s="9"/>
@@ -2997,10 +2836,19 @@
       <c r="H86" s="9"/>
       <c r="I86" s="9"/>
     </row>
-    <row r="87" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-      <c r="I87" s="9"/>
+    <row r="87" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="117" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" s="117"/>
+      <c r="F87" s="118" t="s">
+        <v>99</v>
+      </c>
+      <c r="G87" s="118"/>
+      <c r="H87" s="119" t="s">
+        <v>100</v>
+      </c>
+      <c r="I87" s="119"/>
     </row>
     <row r="88" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G88" s="9"/>
@@ -3008,14 +2856,40 @@
       <c r="I88" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="E64:H64"/>
+  <mergeCells count="56">
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="C81:D85"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="D22:D29"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F23:F28"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="F41:F42"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -3032,35 +2906,13 @@
     <mergeCell ref="E39:E40"/>
     <mergeCell ref="F37:F38"/>
     <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F23:F28"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="G45:G48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="D22:D29"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="E44:E48"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="E64:H64"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Actualización Reporte Boleta Determinación
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB87A65-E870-4984-9155-EE36894BDD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7965174D-2044-41AF-9FD2-9DBA8B771C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
   </bookViews>
@@ -567,10 +567,10 @@
     <t>Representante UNNA ENERGIA-PGT</t>
   </si>
   <si>
-    <t xml:space="preserve">   Representante UNNA ENERGIA-Lote IV</t>
-  </si>
-  <si>
     <t xml:space="preserve">          Representante Perupetro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Representante UNNA ENERGIA-Lote IV</t>
   </si>
 </sst>
 </file>
@@ -1095,20 +1095,74 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1116,33 +1170,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1179,56 +1206,29 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1309,156 +1309,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>201706</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2107013</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>201706</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Conector recto 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67BB32D8-8C00-4B31-B093-892DA6997D2A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="963706" y="20473147"/>
-          <a:ext cx="2700925" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>156882</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>594219</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Conector recto 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6566DD-D73B-4654-8659-E9DDF0290092}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4997823" y="20495559"/>
-          <a:ext cx="2700925" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1994648</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1244161</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Conector recto 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C06FF797-1B9D-4265-8A6F-074F182AC209}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9099177" y="20439529"/>
-          <a:ext cx="2700925" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1848,8 +1698,8 @@
   </sheetPr>
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A59" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A67" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1870,42 +1720,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="91"/>
-      <c r="C1" s="92"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="101"/>
       <c r="D1" s="59"/>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="98"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="107"/>
       <c r="I1" s="58" t="s">
         <v>74</v>
       </c>
       <c r="J1" s="58"/>
     </row>
     <row r="2" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="93"/>
-      <c r="C2" s="94"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="103"/>
       <c r="D2" s="56"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="80" t="s">
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="81"/>
+      <c r="J2" s="99"/>
       <c r="K2" s="55"/>
     </row>
     <row r="3" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="95"/>
-      <c r="C3" s="96"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="105"/>
       <c r="D3" s="54"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="102"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="111"/>
       <c r="I3" s="53" t="s">
         <v>72</v>
       </c>
@@ -1981,13 +1831,13 @@
       <c r="C10" s="48"/>
     </row>
     <row r="11" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="83" t="s">
+      <c r="E11" s="88" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="27" t="s">
@@ -1999,9 +1849,9 @@
     </row>
     <row r="12" spans="2:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="47"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="84"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="90"/>
       <c r="F12" s="19" t="s">
         <v>49</v>
       </c>
@@ -2017,8 +1867,8 @@
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B13" s="47"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
       <c r="E13" s="8" t="s">
         <v>45</v>
       </c>
@@ -2105,14 +1955,14 @@
     <row r="19" spans="1:9" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="104" t="s">
+      <c r="D19" s="96"/>
+      <c r="E19" s="112" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="103" t="s">
+      <c r="F19" s="81" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="17"/>
@@ -2120,23 +1970,23 @@
       <c r="I19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="103"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="81"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D22" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="86" t="s">
+      <c r="E22" s="91" t="s">
         <v>33</v>
       </c>
       <c r="F22" s="27" t="s">
@@ -2147,70 +1997,70 @@
       <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C23" s="82"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="86" t="s">
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="86" t="s">
+      <c r="G23" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="86" t="s">
+      <c r="H23" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="86" t="s">
+      <c r="I23" s="91" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92"/>
+      <c r="I24" s="92"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="92"/>
+      <c r="I27" s="92"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="93"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
       <c r="E29" s="8" t="s">
         <v>45</v>
       </c>
@@ -2301,13 +2151,13 @@
     </row>
     <row r="37" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C37" s="9"/>
-      <c r="D37" s="86" t="s">
+      <c r="D37" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="89" t="s">
+      <c r="E37" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="103" t="s">
+      <c r="F37" s="81" t="s">
         <v>34</v>
       </c>
       <c r="G37" s="28"/>
@@ -2316,22 +2166,22 @@
     </row>
     <row r="38" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C38" s="9"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="103"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="95"/>
+      <c r="F38" s="81"/>
       <c r="G38" s="28"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C39" s="9"/>
-      <c r="D39" s="86" t="s">
+      <c r="D39" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="89" t="s">
+      <c r="E39" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="103" t="s">
+      <c r="F39" s="81" t="s">
         <v>34</v>
       </c>
       <c r="G39" s="28"/>
@@ -2340,22 +2190,22 @@
     </row>
     <row r="40" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C40" s="9"/>
-      <c r="D40" s="88"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="103"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="81"/>
       <c r="G40" s="28"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="9"/>
-      <c r="D41" s="86" t="s">
+      <c r="D41" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="89" t="s">
+      <c r="E41" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="109" t="s">
+      <c r="F41" s="97" t="s">
         <v>34</v>
       </c>
       <c r="G41" s="28"/>
@@ -2364,21 +2214,21 @@
     </row>
     <row r="42" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C42" s="9"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="90"/>
-      <c r="F42" s="109"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="97"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
     <row r="44" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="82" t="s">
+      <c r="C44" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="82" t="s">
+      <c r="D44" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="83" t="s">
+      <c r="E44" s="88" t="s">
         <v>33</v>
       </c>
       <c r="F44" s="27" t="s">
@@ -2389,52 +2239,52 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="85" t="s">
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="85" t="s">
+      <c r="G45" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="H45" s="85" t="s">
+      <c r="H45" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="85" t="s">
+      <c r="I45" s="96" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="46" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="105"/>
-      <c r="F46" s="85"/>
-      <c r="G46" s="85"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="85"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="87"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="96"/>
+      <c r="G46" s="96"/>
+      <c r="H46" s="96"/>
+      <c r="I46" s="96"/>
     </row>
     <row r="47" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="105"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
+      <c r="C47" s="87"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="96"/>
     </row>
     <row r="48" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="84"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
+      <c r="C48" s="87"/>
+      <c r="D48" s="87"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
+      <c r="I48" s="96"/>
     </row>
     <row r="49" spans="3:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
       <c r="E49" s="8" t="s">
         <v>28</v>
       </c>
@@ -2485,11 +2335,11 @@
     </row>
     <row r="52" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C52" s="9"/>
-      <c r="D52" s="116"/>
-      <c r="E52" s="116"/>
-      <c r="F52" s="116"/>
-      <c r="G52" s="116"/>
-      <c r="H52" s="116"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
       <c r="I52" s="14"/>
     </row>
     <row r="53" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2503,13 +2353,13 @@
     <row r="54" spans="3:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="57"/>
       <c r="E54" s="63"/>
-      <c r="G54" s="110" t="s">
+      <c r="G54" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="112" t="s">
+      <c r="H54" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="I54" s="103" t="s">
+      <c r="I54" s="81" t="s">
         <v>21</v>
       </c>
       <c r="L54" s="16"/>
@@ -2517,26 +2367,26 @@
     <row r="55" spans="3:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="57"/>
       <c r="E55" s="63"/>
-      <c r="G55" s="111"/>
-      <c r="H55" s="113"/>
-      <c r="I55" s="103"/>
+      <c r="G55" s="78"/>
+      <c r="H55" s="80"/>
+      <c r="I55" s="81"/>
       <c r="L55" s="16"/>
     </row>
     <row r="56" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G56" s="75" t="s">
+      <c r="G56" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="114" t="s">
+      <c r="H56" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="I56" s="115" t="s">
+      <c r="I56" s="84" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="57" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G57" s="75"/>
-      <c r="H57" s="114"/>
-      <c r="I57" s="115"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="84"/>
     </row>
     <row r="58" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="G58" s="7"/>
@@ -2576,54 +2426,54 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="3:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="C64" s="76" t="s">
+      <c r="C64" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="76" t="s">
+      <c r="D64" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="77" t="s">
+      <c r="E64" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="F64" s="78"/>
-      <c r="G64" s="78"/>
-      <c r="H64" s="79"/>
+      <c r="F64" s="115"/>
+      <c r="G64" s="115"/>
+      <c r="H64" s="116"/>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="76"/>
-      <c r="D65" s="76"/>
-      <c r="E65" s="75" t="s">
+      <c r="C65" s="113"/>
+      <c r="D65" s="113"/>
+      <c r="E65" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="75" t="s">
+      <c r="F65" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="75" t="s">
+      <c r="G65" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="75" t="s">
+      <c r="H65" s="82" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="76"/>
-      <c r="D66" s="76"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
+      <c r="C66" s="113"/>
+      <c r="D66" s="113"/>
+      <c r="E66" s="82"/>
+      <c r="F66" s="82"/>
+      <c r="G66" s="82"/>
+      <c r="H66" s="82"/>
     </row>
     <row r="67" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C67" s="76"/>
-      <c r="D67" s="76"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
+      <c r="C67" s="113"/>
+      <c r="D67" s="113"/>
+      <c r="E67" s="82"/>
+      <c r="F67" s="82"/>
+      <c r="G67" s="82"/>
+      <c r="H67" s="82"/>
     </row>
     <row r="68" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C68" s="76"/>
-      <c r="D68" s="76"/>
+      <c r="C68" s="113"/>
+      <c r="D68" s="113"/>
       <c r="E68" s="6" t="s">
         <v>11</v>
       </c>
@@ -2666,11 +2516,11 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="108" t="s">
+      <c r="B72" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="108"/>
-      <c r="D72" s="108"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="86"/>
       <c r="E72" s="5" t="s">
         <v>85</v>
       </c>
@@ -2696,11 +2546,11 @@
       <c r="H73" s="13"/>
     </row>
     <row r="74" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="108" t="s">
+      <c r="B74" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="108"/>
-      <c r="D74" s="108"/>
+      <c r="C74" s="86"/>
+      <c r="D74" s="86"/>
       <c r="E74" s="5" t="s">
         <v>88</v>
       </c>
@@ -2711,11 +2561,11 @@
       <c r="H74" s="13"/>
     </row>
     <row r="75" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="108" t="s">
+      <c r="B75" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="108"/>
-      <c r="D75" s="108"/>
+      <c r="C75" s="86"/>
+      <c r="D75" s="86"/>
       <c r="E75" s="5" t="s">
         <v>87</v>
       </c>
@@ -2726,11 +2576,11 @@
       <c r="H75" s="13"/>
     </row>
     <row r="76" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="108" t="s">
+      <c r="B76" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="108"/>
-      <c r="D76" s="108"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="86"/>
       <c r="E76" s="5" t="s">
         <v>89</v>
       </c>
@@ -2745,10 +2595,10 @@
       <c r="G77" s="12"/>
     </row>
     <row r="78" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="106" t="s">
+      <c r="C78" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="106"/>
+      <c r="D78" s="85"/>
       <c r="E78" s="64" t="s">
         <v>90</v>
       </c>
@@ -2760,10 +2610,10 @@
       <c r="I78" s="9"/>
     </row>
     <row r="79" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C79" s="107" t="s">
+      <c r="C79" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D79" s="107"/>
+      <c r="D79" s="76"/>
       <c r="E79" s="65" t="s">
         <v>91</v>
       </c>
@@ -2783,113 +2633,89 @@
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
     </row>
-    <row r="81" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C81" s="107" t="e" vm="1">
+    <row r="81" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C81" s="76" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="D81" s="107"/>
+      <c r="D81" s="76"/>
       <c r="E81" s="65"/>
       <c r="F81" s="2"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
     </row>
-    <row r="82" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C82" s="107"/>
-      <c r="D82" s="107"/>
+    <row r="82" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C82" s="76"/>
+      <c r="D82" s="76"/>
       <c r="E82" s="65"/>
       <c r="F82" s="2"/>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
       <c r="I82" s="9"/>
     </row>
-    <row r="83" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C83" s="107"/>
-      <c r="D83" s="107"/>
+    <row r="83" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C83" s="76"/>
+      <c r="D83" s="76"/>
       <c r="E83" s="65"/>
       <c r="F83" s="2"/>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
     </row>
-    <row r="84" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C84" s="107"/>
-      <c r="D84" s="107"/>
+    <row r="84" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C84" s="76"/>
+      <c r="D84" s="76"/>
       <c r="E84" s="65"/>
       <c r="F84" s="2"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
     </row>
-    <row r="85" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C85" s="107"/>
-      <c r="D85" s="107"/>
+    <row r="85" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C85" s="76"/>
+      <c r="D85" s="76"/>
       <c r="E85" s="65"/>
       <c r="F85" s="2"/>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
       <c r="I85" s="9"/>
     </row>
-    <row r="86" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E86" s="67"/>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
       <c r="I86" s="9"/>
     </row>
-    <row r="87" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C87" s="117" t="s">
         <v>98</v>
       </c>
       <c r="D87" s="117"/>
       <c r="F87" s="118" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G87" s="118"/>
       <c r="H87" s="119" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I87" s="119"/>
-    </row>
-    <row r="88" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J87" s="119"/>
+    </row>
+    <row r="88" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
       <c r="I88" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="D52:H52"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="C81:D85"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="D22:D29"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="E44:E48"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F23:F28"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="G45:G48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="D64:D68"/>
+    <mergeCell ref="E64:H64"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="D11:D13"/>
@@ -2906,13 +2732,38 @@
     <mergeCell ref="E39:E40"/>
     <mergeCell ref="F37:F38"/>
     <mergeCell ref="F39:F40"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="D64:D68"/>
-    <mergeCell ref="E64:H64"/>
+    <mergeCell ref="F23:F28"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="D22:D29"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="C81:D85"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
Actualización de PDF IText
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7965174D-2044-41AF-9FD2-9DBA8B771C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88C5961-D660-42EC-AC7D-FC41F1B558A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
   </bookViews>
@@ -1095,9 +1095,117 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1113,12 +1221,6 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1127,108 +1229,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1699,7 +1699,7 @@
   <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A67" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1720,42 +1720,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="100"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="93"/>
       <c r="D1" s="59"/>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="99"/>
       <c r="I1" s="58" t="s">
         <v>74</v>
       </c>
       <c r="J1" s="58"/>
     </row>
     <row r="2" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="102"/>
-      <c r="C2" s="103"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="95"/>
       <c r="D2" s="56"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="98" t="s">
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="J2" s="99"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="55"/>
     </row>
     <row r="3" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="104"/>
-      <c r="C3" s="105"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="97"/>
       <c r="D3" s="54"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="111"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103"/>
       <c r="I3" s="53" t="s">
         <v>72</v>
       </c>
@@ -1831,13 +1831,13 @@
       <c r="C10" s="48"/>
     </row>
     <row r="11" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="84" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="27" t="s">
@@ -1849,9 +1849,9 @@
     </row>
     <row r="12" spans="2:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="47"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="90"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="85"/>
       <c r="F12" s="19" t="s">
         <v>49</v>
       </c>
@@ -1867,8 +1867,8 @@
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B13" s="47"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="8" t="s">
         <v>45</v>
       </c>
@@ -1955,14 +1955,14 @@
     <row r="19" spans="1:9" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="96" t="s">
+      <c r="C19" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="96"/>
-      <c r="E19" s="112" t="s">
+      <c r="D19" s="86"/>
+      <c r="E19" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="81" t="s">
+      <c r="F19" s="104" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="17"/>
@@ -1970,23 +1970,23 @@
       <c r="I19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="81"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="104"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="87" t="s">
+      <c r="D22" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="91" t="s">
+      <c r="E22" s="87" t="s">
         <v>33</v>
       </c>
       <c r="F22" s="27" t="s">
@@ -1997,70 +1997,70 @@
       <c r="I22" s="26"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="91" t="s">
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="91" t="s">
+      <c r="G23" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="91" t="s">
+      <c r="H23" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="91" t="s">
+      <c r="I23" s="87" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C26" s="87"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="92"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="92"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="93"/>
-      <c r="I28" s="93"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
       <c r="E29" s="8" t="s">
         <v>45</v>
       </c>
@@ -2151,13 +2151,13 @@
     </row>
     <row r="37" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C37" s="9"/>
-      <c r="D37" s="91" t="s">
+      <c r="D37" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="94" t="s">
+      <c r="E37" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="F37" s="81" t="s">
+      <c r="F37" s="104" t="s">
         <v>34</v>
       </c>
       <c r="G37" s="28"/>
@@ -2166,22 +2166,22 @@
     </row>
     <row r="38" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C38" s="9"/>
-      <c r="D38" s="93"/>
-      <c r="E38" s="95"/>
-      <c r="F38" s="81"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="91"/>
+      <c r="F38" s="104"/>
       <c r="G38" s="28"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C39" s="9"/>
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="94" t="s">
+      <c r="E39" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="81" t="s">
+      <c r="F39" s="104" t="s">
         <v>34</v>
       </c>
       <c r="G39" s="28"/>
@@ -2190,22 +2190,22 @@
     </row>
     <row r="40" spans="3:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C40" s="9"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="95"/>
-      <c r="F40" s="81"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="91"/>
+      <c r="F40" s="104"/>
       <c r="G40" s="28"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="9"/>
-      <c r="D41" s="91" t="s">
+      <c r="D41" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="94" t="s">
+      <c r="E41" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="97" t="s">
+      <c r="F41" s="106" t="s">
         <v>34</v>
       </c>
       <c r="G41" s="28"/>
@@ -2214,21 +2214,21 @@
     </row>
     <row r="42" spans="3:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C42" s="9"/>
-      <c r="D42" s="93"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="97"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="106"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
     <row r="44" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="87" t="s">
+      <c r="C44" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="87" t="s">
+      <c r="D44" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="88" t="s">
+      <c r="E44" s="84" t="s">
         <v>33</v>
       </c>
       <c r="F44" s="27" t="s">
@@ -2239,52 +2239,52 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="96" t="s">
+      <c r="C45" s="83"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="107"/>
+      <c r="F45" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="96" t="s">
+      <c r="G45" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="H45" s="96" t="s">
+      <c r="H45" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="96" t="s">
+      <c r="I45" s="86" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="46" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="87"/>
-      <c r="D46" s="87"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="96"/>
-      <c r="G46" s="96"/>
-      <c r="H46" s="96"/>
-      <c r="I46" s="96"/>
+      <c r="C46" s="83"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="107"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="86"/>
     </row>
     <row r="47" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="87"/>
-      <c r="D47" s="87"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="96"/>
-      <c r="G47" s="96"/>
-      <c r="H47" s="96"/>
-      <c r="I47" s="96"/>
+      <c r="C47" s="83"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="86"/>
+      <c r="G47" s="86"/>
+      <c r="H47" s="86"/>
+      <c r="I47" s="86"/>
     </row>
     <row r="48" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C48" s="87"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="96"/>
-      <c r="H48" s="96"/>
-      <c r="I48" s="96"/>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="86"/>
+      <c r="G48" s="86"/>
+      <c r="H48" s="86"/>
+      <c r="I48" s="86"/>
     </row>
     <row r="49" spans="3:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="C49" s="87"/>
-      <c r="D49" s="87"/>
+      <c r="C49" s="83"/>
+      <c r="D49" s="83"/>
       <c r="E49" s="8" t="s">
         <v>28</v>
       </c>
@@ -2335,11 +2335,11 @@
     </row>
     <row r="52" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="C52" s="9"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
+      <c r="D52" s="109"/>
+      <c r="E52" s="109"/>
+      <c r="F52" s="109"/>
+      <c r="G52" s="109"/>
+      <c r="H52" s="109"/>
       <c r="I52" s="14"/>
     </row>
     <row r="53" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2353,13 +2353,13 @@
     <row r="54" spans="3:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="57"/>
       <c r="E54" s="63"/>
-      <c r="G54" s="77" t="s">
+      <c r="G54" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="79" t="s">
+      <c r="H54" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="I54" s="81" t="s">
+      <c r="I54" s="104" t="s">
         <v>21</v>
       </c>
       <c r="L54" s="16"/>
@@ -2367,26 +2367,26 @@
     <row r="55" spans="3:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="57"/>
       <c r="E55" s="63"/>
-      <c r="G55" s="78"/>
-      <c r="H55" s="80"/>
-      <c r="I55" s="81"/>
+      <c r="G55" s="114"/>
+      <c r="H55" s="116"/>
+      <c r="I55" s="104"/>
       <c r="L55" s="16"/>
     </row>
     <row r="56" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G56" s="82" t="s">
+      <c r="G56" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="83" t="s">
+      <c r="H56" s="117" t="s">
         <v>82</v>
       </c>
-      <c r="I56" s="84" t="s">
+      <c r="I56" s="118" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="57" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G57" s="82"/>
-      <c r="H57" s="83"/>
-      <c r="I57" s="84"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="117"/>
+      <c r="I57" s="118"/>
     </row>
     <row r="58" spans="3:12" ht="15" x14ac:dyDescent="0.2">
       <c r="G58" s="7"/>
@@ -2426,54 +2426,54 @@
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="3:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="C64" s="113" t="s">
+      <c r="C64" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="113" t="s">
+      <c r="D64" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="114" t="s">
+      <c r="E64" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F64" s="115"/>
-      <c r="G64" s="115"/>
-      <c r="H64" s="116"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="79"/>
+      <c r="H64" s="80"/>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="113"/>
-      <c r="D65" s="113"/>
-      <c r="E65" s="82" t="s">
+      <c r="C65" s="77"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="82" t="s">
+      <c r="F65" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="82" t="s">
+      <c r="G65" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="H65" s="82" t="s">
+      <c r="H65" s="76" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="66" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="113"/>
-      <c r="D66" s="113"/>
-      <c r="E66" s="82"/>
-      <c r="F66" s="82"/>
-      <c r="G66" s="82"/>
-      <c r="H66" s="82"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="76"/>
     </row>
     <row r="67" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C67" s="113"/>
-      <c r="D67" s="113"/>
-      <c r="E67" s="82"/>
-      <c r="F67" s="82"/>
-      <c r="G67" s="82"/>
-      <c r="H67" s="82"/>
+      <c r="C67" s="77"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="76"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="76"/>
     </row>
     <row r="68" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C68" s="113"/>
-      <c r="D68" s="113"/>
+      <c r="C68" s="77"/>
+      <c r="D68" s="77"/>
       <c r="E68" s="6" t="s">
         <v>11</v>
       </c>
@@ -2516,11 +2516,11 @@
       <c r="H71" s="13"/>
     </row>
     <row r="72" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="86" t="s">
+      <c r="B72" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="86"/>
-      <c r="D72" s="86"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="108"/>
       <c r="E72" s="5" t="s">
         <v>85</v>
       </c>
@@ -2546,11 +2546,11 @@
       <c r="H73" s="13"/>
     </row>
     <row r="74" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="86" t="s">
+      <c r="B74" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="86"/>
-      <c r="D74" s="86"/>
+      <c r="C74" s="108"/>
+      <c r="D74" s="108"/>
       <c r="E74" s="5" t="s">
         <v>88</v>
       </c>
@@ -2561,11 +2561,11 @@
       <c r="H74" s="13"/>
     </row>
     <row r="75" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="86" t="s">
+      <c r="B75" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="86"/>
-      <c r="D75" s="86"/>
+      <c r="C75" s="108"/>
+      <c r="D75" s="108"/>
       <c r="E75" s="5" t="s">
         <v>87</v>
       </c>
@@ -2576,11 +2576,11 @@
       <c r="H75" s="13"/>
     </row>
     <row r="76" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="86" t="s">
+      <c r="B76" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="86"/>
-      <c r="D76" s="86"/>
+      <c r="C76" s="108"/>
+      <c r="D76" s="108"/>
       <c r="E76" s="5" t="s">
         <v>89</v>
       </c>
@@ -2595,10 +2595,10 @@
       <c r="G77" s="12"/>
     </row>
     <row r="78" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="85" t="s">
+      <c r="C78" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="85"/>
+      <c r="D78" s="119"/>
       <c r="E78" s="64" t="s">
         <v>90</v>
       </c>
@@ -2610,10 +2610,10 @@
       <c r="I78" s="9"/>
     </row>
     <row r="79" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C79" s="76" t="s">
+      <c r="C79" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="D79" s="76"/>
+      <c r="D79" s="112"/>
       <c r="E79" s="65" t="s">
         <v>91</v>
       </c>
@@ -2634,10 +2634,10 @@
       <c r="I80" s="9"/>
     </row>
     <row r="81" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C81" s="76" t="e" vm="1">
+      <c r="C81" s="112" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="D81" s="76"/>
+      <c r="D81" s="112"/>
       <c r="E81" s="65"/>
       <c r="F81" s="2"/>
       <c r="G81" s="9"/>
@@ -2645,8 +2645,8 @@
       <c r="I81" s="9"/>
     </row>
     <row r="82" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C82" s="76"/>
-      <c r="D82" s="76"/>
+      <c r="C82" s="112"/>
+      <c r="D82" s="112"/>
       <c r="E82" s="65"/>
       <c r="F82" s="2"/>
       <c r="G82" s="9"/>
@@ -2654,8 +2654,8 @@
       <c r="I82" s="9"/>
     </row>
     <row r="83" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C83" s="76"/>
-      <c r="D83" s="76"/>
+      <c r="C83" s="112"/>
+      <c r="D83" s="112"/>
       <c r="E83" s="65"/>
       <c r="F83" s="2"/>
       <c r="G83" s="9"/>
@@ -2663,8 +2663,8 @@
       <c r="I83" s="9"/>
     </row>
     <row r="84" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C84" s="76"/>
-      <c r="D84" s="76"/>
+      <c r="C84" s="112"/>
+      <c r="D84" s="112"/>
       <c r="E84" s="65"/>
       <c r="F84" s="2"/>
       <c r="G84" s="9"/>
@@ -2672,8 +2672,8 @@
       <c r="I84" s="9"/>
     </row>
     <row r="85" spans="3:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C85" s="76"/>
-      <c r="D85" s="76"/>
+      <c r="C85" s="112"/>
+      <c r="D85" s="112"/>
       <c r="E85" s="65"/>
       <c r="F85" s="2"/>
       <c r="G85" s="9"/>
@@ -2687,19 +2687,19 @@
       <c r="I86" s="9"/>
     </row>
     <row r="87" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="117" t="s">
+      <c r="C87" s="110" t="s">
         <v>98</v>
       </c>
-      <c r="D87" s="117"/>
-      <c r="F87" s="118" t="s">
+      <c r="D87" s="110"/>
+      <c r="F87" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="G87" s="118"/>
-      <c r="H87" s="119" t="s">
+      <c r="G87" s="111"/>
+      <c r="H87" s="75" t="s">
         <v>99</v>
       </c>
-      <c r="I87" s="119"/>
-      <c r="J87" s="119"/>
+      <c r="I87" s="75"/>
+      <c r="J87" s="75"/>
     </row>
     <row r="88" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G88" s="9"/>
@@ -2708,11 +2708,41 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="H87:J87"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="C81:D85"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="D22:D29"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="D44:D49"/>
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="E44:E48"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F23:F28"/>
+    <mergeCell ref="G23:G28"/>
     <mergeCell ref="C64:C68"/>
     <mergeCell ref="D64:D68"/>
     <mergeCell ref="E64:H64"/>
@@ -2729,44 +2759,14 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F23:F28"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="G45:G48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="E44:E48"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="C22:C29"/>
-    <mergeCell ref="D22:D29"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="D44:D49"/>
-    <mergeCell ref="D52:H52"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="C81:D85"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="H65:H67"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>
+  <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0" header="0.15748031496062992" footer="0.15748031496062992"/>
   <pageSetup paperSize="9" scale="43" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <colBreaks count="1" manualBreakCount="1">

</xml_diff>

<commit_message>
subir cambios de reportes
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnnaReportesOperativos3\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17343766-603D-459D-991D-D09C21BE191D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7689DAD3-06ED-4E43-A533-73D90929B36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Boleta_CNPC" sheetId="3" r:id="rId1"/>
@@ -37,155 +37,6 @@
     <author>Jean Cabrera</author>
   </authors>
   <commentList>
-    <comment ref="D67" authorId="0" shapeId="0" xr:uid="{24F11996-FE51-4DFF-99E3-A2E2E1CE98D4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jean Cabrera:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Valor = Volumen de GNS a venta (ENEL + GASNORP + Limagas)
-Considerar 4 decimales</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D68" authorId="0" shapeId="0" xr:uid="{AA2054F2-082B-4CAF-8F53-4209463F78C4}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jean Cabrera:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-GNS VENTA UNNA (LOTE IV) del segundo registro, IdDato 6 de la tabla Dato de la BD</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{87946FD7-BEAE-4AFA-98F6-AA911D282337}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jean Cabrera:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dato suministrado por el Supervisor PGT
-Considerar 4 decimales, CELDA G26</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D70" authorId="0" shapeId="0" xr:uid="{F953D711-3E7F-45B7-A85E-CB966DB833BA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jean Cabrera:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Dato suministrado por el Supervisor PGT
-Considerar 4 decimales, celda g25</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D71" authorId="0" shapeId="0" xr:uid="{3345D229-E972-4BC2-8948-C33044D31E6B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jean Cabrera:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Valor = Volumen de GNSd de UNNA ENERGIA LOTE IV (D73) - Volumen de GNS a venta Total (D76)
-Considerar 4 decimales</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D73" authorId="0" shapeId="0" xr:uid="{6AE12449-5371-4D22-AE57-E9E8844F9F78}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jean Cabrera:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Valor = Gas Combustible (E73) + Volumen de GNS equiv. de LGN (F73)
-Considerar 4 decimales</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="D74" authorId="0" shapeId="0" xr:uid="{DB6E7D09-DC3A-49EB-B995-3B2A33976217}">
       <text>
         <r>
@@ -216,14 +67,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
           <xlrd:rvb i="0"/>
         </ext>
       </extLst>
@@ -575,7 +426,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1126,12 +977,175 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1149,169 +1163,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1396,7 +1247,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1781,67 +1632,67 @@
   </sheetPr>
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="5.625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="10" customWidth="1"/>
+    <col min="3" max="3" width="52.375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="33.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="22.125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="25.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="20.875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="20.25" style="9" customWidth="1"/>
     <col min="11" max="11" width="4" style="9"/>
-    <col min="12" max="12" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.25" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="4" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113"/>
-      <c r="B1" s="114"/>
+    <row r="1" spans="1:11" ht="21.75" customHeight="1">
+      <c r="A1" s="110"/>
+      <c r="B1" s="111"/>
       <c r="C1" s="56"/>
-      <c r="D1" s="119" t="s">
+      <c r="D1" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="120"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="117"/>
       <c r="I1" s="55" t="s">
         <v>71</v>
       </c>
       <c r="J1" s="55"/>
     </row>
-    <row r="2" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115"/>
-      <c r="B2" s="116"/>
+    <row r="2" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A2" s="112"/>
+      <c r="B2" s="113"/>
       <c r="C2" s="53"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="111" t="s">
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="112"/>
+      <c r="J2" s="102"/>
       <c r="K2" s="52"/>
     </row>
-    <row r="3" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117"/>
-      <c r="B3" s="118"/>
+    <row r="3" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A3" s="114"/>
+      <c r="B3" s="115"/>
       <c r="C3" s="51"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="124"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="121"/>
       <c r="I3" s="74" t="s">
         <v>97</v>
       </c>
@@ -1849,10 +1700,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="32.25" customHeight="1">
       <c r="A4" s="45"/>
     </row>
-    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="31.5" customHeight="1">
       <c r="A5" s="45"/>
       <c r="B5" s="9"/>
       <c r="C5" s="11"/>
@@ -1867,7 +1718,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="31.5" customHeight="1">
       <c r="A6" s="45"/>
       <c r="B6" s="9"/>
       <c r="C6" s="30"/>
@@ -1878,7 +1729,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="49"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="45"/>
       <c r="B7" s="30" t="s">
         <v>56</v>
@@ -1891,7 +1742,7 @@
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8" s="45"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -1901,7 +1752,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="47"/>
     </row>
-    <row r="9" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="27.75" customHeight="1">
       <c r="A9" s="45"/>
       <c r="B9" s="9"/>
       <c r="C9" s="15" t="s">
@@ -1918,17 +1769,17 @@
       <c r="H9" s="57"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="10" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="22.5" customHeight="1">
       <c r="B10" s="46"/>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="110" t="s">
+    <row r="11" spans="1:11" ht="15">
+      <c r="B11" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="103" t="s">
+      <c r="D11" s="104" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="26" t="s">
@@ -1939,18 +1790,18 @@
       <c r="H11" s="26"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="60">
       <c r="A12" s="45"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="103"/>
       <c r="D12" s="105"/>
       <c r="E12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="148" t="s">
+      <c r="F12" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="149"/>
+      <c r="G12" s="94"/>
       <c r="H12" s="18" t="s">
         <v>47</v>
       </c>
@@ -1958,20 +1809,20 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75">
       <c r="A13" s="45"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="135" t="s">
+      <c r="F13" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="136"/>
+      <c r="G13" s="96"/>
       <c r="H13" s="6" t="s">
         <v>42</v>
       </c>
@@ -1979,7 +1830,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75">
       <c r="A14" s="45"/>
       <c r="B14" s="37" t="s">
         <v>63</v>
@@ -1993,10 +1844,10 @@
       <c r="E14" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="137" t="s">
+      <c r="F14" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="138"/>
+      <c r="G14" s="98"/>
       <c r="H14" s="34" t="s">
         <v>75</v>
       </c>
@@ -2005,18 +1856,18 @@
       </c>
       <c r="J14" s="40"/>
     </row>
-    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="18" customHeight="1">
       <c r="B15" s="37"/>
       <c r="C15" s="32"/>
       <c r="D15" s="35"/>
       <c r="E15" s="34"/>
-      <c r="F15" s="150"/>
-      <c r="G15" s="151"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="100"/>
       <c r="H15" s="34"/>
       <c r="I15" s="33"/>
       <c r="J15" s="40"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="B16" s="17"/>
       <c r="D16" s="44"/>
       <c r="E16" s="42"/>
@@ -2026,7 +1877,7 @@
       <c r="I16" s="41"/>
       <c r="J16" s="40"/>
     </row>
-    <row r="17" spans="1:9" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="38" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="39"/>
       <c r="C17" s="17"/>
@@ -2039,7 +1890,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="1:9" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="39"/>
       <c r="C18" s="17"/>
@@ -2049,32 +1900,32 @@
       <c r="H18" s="17"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="1:9" s="38" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="38" customFormat="1" ht="20.25" customHeight="1">
       <c r="A19" s="9"/>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="109"/>
+      <c r="C19" s="106"/>
       <c r="D19" s="77" t="s">
         <v>77</v>
       </c>
       <c r="E19" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="125"/>
+      <c r="F19" s="89"/>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="30"/>
     </row>
-    <row r="20" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="110" t="s">
+    <row r="20" spans="1:9" ht="33" customHeight="1"/>
+    <row r="21" spans="1:9" ht="18" customHeight="1">
+      <c r="B21" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="110" t="s">
+      <c r="C21" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="106" t="s">
+      <c r="D21" s="107" t="s">
         <v>33</v>
       </c>
       <c r="E21" s="26" t="s">
@@ -2085,67 +1936,67 @@
       <c r="H21" s="26"/>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="110"/>
-      <c r="C22" s="110"/>
-      <c r="D22" s="107"/>
-      <c r="E22" s="106" t="s">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="139" t="s">
+      <c r="F22" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="103"/>
-      <c r="H22" s="106" t="s">
+      <c r="G22" s="104"/>
+      <c r="H22" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="106" t="s">
+      <c r="I22" s="107" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="110"/>
-      <c r="C23" s="110"/>
-      <c r="D23" s="107"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="140"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="107"/>
-      <c r="I23" s="107"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="110"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="140"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="110"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="108"/>
-      <c r="E25" s="108"/>
-      <c r="F25" s="141"/>
+    <row r="23" spans="1:9" ht="15">
+      <c r="B23" s="103"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="123"/>
+      <c r="G23" s="124"/>
+      <c r="H23" s="108"/>
+      <c r="I23" s="108"/>
+    </row>
+    <row r="24" spans="1:9" ht="15">
+      <c r="B24" s="103"/>
+      <c r="C24" s="103"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="123"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="108"/>
+    </row>
+    <row r="25" spans="1:9" ht="15">
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="109"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="125"/>
       <c r="G25" s="105"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="108"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="110"/>
-      <c r="C26" s="110"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
       <c r="D26" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="135" t="s">
+      <c r="F26" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="136"/>
+      <c r="G26" s="96"/>
       <c r="H26" s="6" t="s">
         <v>42</v>
       </c>
@@ -2153,7 +2004,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="B27" s="37" t="s">
         <v>63</v>
       </c>
@@ -2166,10 +2017,10 @@
       <c r="E27" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="137" t="s">
+      <c r="F27" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="138"/>
+      <c r="G27" s="98"/>
       <c r="H27" s="34" t="s">
         <v>75</v>
       </c>
@@ -2177,17 +2028,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="23.25" customHeight="1">
       <c r="B28" s="32"/>
       <c r="C28" s="20"/>
       <c r="D28" s="23"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="147"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="132"/>
       <c r="H28" s="31"/>
       <c r="I28" s="22"/>
     </row>
-    <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="18" customHeight="1">
       <c r="C29" s="38"/>
       <c r="D29" s="58"/>
       <c r="E29" s="59"/>
@@ -2196,7 +2047,7 @@
       <c r="H29" s="59"/>
       <c r="I29" s="57"/>
     </row>
-    <row r="30" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="25.5" customHeight="1">
       <c r="B30" s="65" t="s">
         <v>40</v>
       </c>
@@ -2210,7 +2061,7 @@
       <c r="H30" s="59"/>
       <c r="I30" s="57"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15">
       <c r="B31" s="65"/>
       <c r="C31" s="38"/>
       <c r="D31" s="58"/>
@@ -2220,8 +2071,8 @@
       <c r="H31" s="59"/>
       <c r="I31" s="57"/>
     </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15"/>
+    <row r="33" spans="2:12" ht="15">
       <c r="B33" s="30" t="s">
         <v>38</v>
       </c>
@@ -2233,7 +2084,7 @@
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
     </row>
-    <row r="34" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" ht="15">
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="9"/>
@@ -2242,7 +2093,7 @@
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15.75">
       <c r="B35" s="9"/>
       <c r="C35" s="70" t="s">
         <v>37</v>
@@ -2253,12 +2104,12 @@
       <c r="E35" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="F35" s="125"/>
+      <c r="F35" s="89"/>
       <c r="G35" s="27"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15.75">
       <c r="B36" s="9"/>
       <c r="C36" s="70" t="s">
         <v>36</v>
@@ -2269,12 +2120,12 @@
       <c r="E36" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="125"/>
+      <c r="F36" s="89"/>
       <c r="G36" s="27"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="18" customHeight="1">
       <c r="B37" s="9"/>
       <c r="C37" s="15" t="s">
         <v>35</v>
@@ -2285,19 +2136,19 @@
       <c r="E37" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="F37" s="126"/>
+      <c r="F37" s="90"/>
       <c r="G37" s="27"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
     </row>
-    <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="110" t="s">
+    <row r="39" spans="2:12" ht="18" customHeight="1">
+      <c r="B39" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="110" t="s">
+      <c r="C39" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="103" t="s">
+      <c r="D39" s="104" t="s">
         <v>33</v>
       </c>
       <c r="E39" s="26" t="s">
@@ -2308,67 +2159,67 @@
       <c r="H39" s="26"/>
       <c r="I39" s="25"/>
     </row>
-    <row r="40" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="110"/>
-      <c r="C40" s="110"/>
-      <c r="D40" s="104"/>
-      <c r="E40" s="109" t="s">
+    <row r="40" spans="2:12" ht="18" customHeight="1">
+      <c r="B40" s="103"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="124"/>
+      <c r="E40" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="139" t="s">
+      <c r="F40" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="G40" s="103"/>
-      <c r="H40" s="109" t="s">
+      <c r="G40" s="104"/>
+      <c r="H40" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="109" t="s">
+      <c r="I40" s="106" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="110"/>
-      <c r="C41" s="110"/>
-      <c r="D41" s="104"/>
-      <c r="E41" s="109"/>
-      <c r="F41" s="140"/>
-      <c r="G41" s="104"/>
-      <c r="H41" s="109"/>
-      <c r="I41" s="109"/>
-    </row>
-    <row r="42" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="110"/>
-      <c r="C42" s="110"/>
-      <c r="D42" s="104"/>
-      <c r="E42" s="109"/>
-      <c r="F42" s="140"/>
-      <c r="G42" s="104"/>
-      <c r="H42" s="109"/>
-      <c r="I42" s="109"/>
-    </row>
-    <row r="43" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="110"/>
-      <c r="C43" s="110"/>
+    <row r="41" spans="2:12" ht="18" customHeight="1">
+      <c r="B41" s="103"/>
+      <c r="C41" s="103"/>
+      <c r="D41" s="124"/>
+      <c r="E41" s="106"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="124"/>
+      <c r="H41" s="106"/>
+      <c r="I41" s="106"/>
+    </row>
+    <row r="42" spans="2:12" ht="18" customHeight="1">
+      <c r="B42" s="103"/>
+      <c r="C42" s="103"/>
+      <c r="D42" s="124"/>
+      <c r="E42" s="106"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="124"/>
+      <c r="H42" s="106"/>
+      <c r="I42" s="106"/>
+    </row>
+    <row r="43" spans="2:12" ht="15">
+      <c r="B43" s="103"/>
+      <c r="C43" s="103"/>
       <c r="D43" s="105"/>
-      <c r="E43" s="109"/>
-      <c r="F43" s="141"/>
+      <c r="E43" s="106"/>
+      <c r="F43" s="125"/>
       <c r="G43" s="105"/>
-      <c r="H43" s="109"/>
-      <c r="I43" s="109"/>
-    </row>
-    <row r="44" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="110"/>
-      <c r="C44" s="110"/>
+      <c r="H43" s="106"/>
+      <c r="I43" s="106"/>
+    </row>
+    <row r="44" spans="2:12" ht="15.75" customHeight="1">
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
       <c r="D44" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="135" t="s">
+      <c r="F44" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="G44" s="136"/>
+      <c r="G44" s="96"/>
       <c r="H44" s="6" t="s">
         <v>25</v>
       </c>
@@ -2376,7 +2227,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15.75" customHeight="1">
       <c r="B45" s="21" t="s">
         <v>63</v>
       </c>
@@ -2389,10 +2240,10 @@
       <c r="E45" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="F45" s="142" t="s">
+      <c r="F45" s="127" t="s">
         <v>59</v>
       </c>
-      <c r="G45" s="143"/>
+      <c r="G45" s="128"/>
       <c r="H45" s="79" t="s">
         <v>75</v>
       </c>
@@ -2400,27 +2251,27 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15">
       <c r="B46" s="21"/>
       <c r="C46" s="20"/>
       <c r="D46" s="67"/>
       <c r="E46" s="68"/>
-      <c r="F46" s="144"/>
-      <c r="G46" s="145"/>
+      <c r="F46" s="129"/>
+      <c r="G46" s="130"/>
       <c r="H46" s="66"/>
       <c r="I46" s="66"/>
     </row>
-    <row r="47" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:12" ht="15">
       <c r="B47" s="9"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="102"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="102"/>
-      <c r="H47" s="102"/>
+      <c r="C47" s="126"/>
+      <c r="D47" s="126"/>
+      <c r="E47" s="126"/>
+      <c r="F47" s="126"/>
+      <c r="G47" s="126"/>
+      <c r="H47" s="126"/>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:12" ht="18" customHeight="1">
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -2429,53 +2280,53 @@
       <c r="H48" s="9"/>
       <c r="L48" s="16"/>
     </row>
-    <row r="49" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:12" ht="20.25" customHeight="1">
       <c r="C49" s="54"/>
       <c r="D49" s="60"/>
-      <c r="F49" s="90" t="s">
+      <c r="F49" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="G49" s="90"/>
-      <c r="H49" s="99" t="s">
+      <c r="G49" s="138"/>
+      <c r="H49" s="135" t="s">
         <v>78</v>
       </c>
-      <c r="I49" s="89" t="s">
+      <c r="I49" s="145" t="s">
         <v>21</v>
       </c>
       <c r="L49" s="16"/>
     </row>
-    <row r="50" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:12" ht="20.25" customHeight="1">
       <c r="C50" s="54"/>
       <c r="D50" s="60"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="89"/>
+      <c r="F50" s="138"/>
+      <c r="G50" s="138"/>
+      <c r="H50" s="136"/>
+      <c r="I50" s="145"/>
       <c r="L50" s="16"/>
     </row>
-    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F51" s="90" t="s">
+    <row r="51" spans="2:12" ht="18" customHeight="1">
+      <c r="F51" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="G51" s="90"/>
-      <c r="H51" s="91" t="s">
+      <c r="G51" s="138"/>
+      <c r="H51" s="146" t="s">
         <v>79</v>
       </c>
-      <c r="I51" s="92" t="s">
+      <c r="I51" s="147" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F52" s="90"/>
-      <c r="G52" s="90"/>
-      <c r="H52" s="91"/>
-      <c r="I52" s="92"/>
-    </row>
-    <row r="53" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:12" ht="18" customHeight="1">
+      <c r="F52" s="138"/>
+      <c r="G52" s="138"/>
+      <c r="H52" s="146"/>
+      <c r="I52" s="147"/>
+    </row>
+    <row r="53" spans="2:12" ht="15">
       <c r="G53" s="7"/>
       <c r="H53" s="13"/>
     </row>
-    <row r="54" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:12" ht="15">
       <c r="G54" s="3" t="s">
         <v>20</v>
       </c>
@@ -2486,11 +2337,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:12" ht="15">
       <c r="G55" s="14"/>
       <c r="H55" s="13"/>
     </row>
-    <row r="56" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:12" ht="15">
       <c r="B56" s="9"/>
       <c r="C56" s="39" t="s">
         <v>81</v>
@@ -2501,82 +2352,82 @@
       <c r="G56" s="30"/>
       <c r="H56" s="30"/>
     </row>
-    <row r="57" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:12" ht="15">
       <c r="G57" s="14"/>
       <c r="H57" s="13"/>
     </row>
-    <row r="58" spans="2:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:12" ht="15">
       <c r="G58" s="14"/>
       <c r="H58" s="13"/>
     </row>
-    <row r="59" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B59" s="93" t="s">
+    <row r="59" spans="2:12" ht="15">
+      <c r="B59" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="93" t="s">
+      <c r="C59" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="94" t="s">
+      <c r="D59" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="95"/>
-      <c r="F59" s="95"/>
-      <c r="G59" s="95"/>
-      <c r="H59" s="96"/>
-    </row>
-    <row r="60" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="93"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="90" t="s">
+      <c r="E59" s="150"/>
+      <c r="F59" s="150"/>
+      <c r="G59" s="150"/>
+      <c r="H59" s="151"/>
+    </row>
+    <row r="60" spans="2:12" ht="15.75" customHeight="1">
+      <c r="B60" s="148"/>
+      <c r="C60" s="148"/>
+      <c r="D60" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="90" t="s">
+      <c r="E60" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="129" t="s">
+      <c r="F60" s="139" t="s">
         <v>13</v>
       </c>
-      <c r="G60" s="130"/>
-      <c r="H60" s="90" t="s">
+      <c r="G60" s="140"/>
+      <c r="H60" s="138" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="93"/>
-      <c r="C61" s="93"/>
-      <c r="D61" s="90"/>
-      <c r="E61" s="90"/>
-      <c r="F61" s="131"/>
-      <c r="G61" s="132"/>
-      <c r="H61" s="90"/>
-    </row>
-    <row r="62" spans="2:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B62" s="93"/>
-      <c r="C62" s="93"/>
-      <c r="D62" s="90"/>
-      <c r="E62" s="90"/>
-      <c r="F62" s="133"/>
-      <c r="G62" s="134"/>
-      <c r="H62" s="90"/>
-    </row>
-    <row r="63" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="93"/>
-      <c r="C63" s="93"/>
+    <row r="61" spans="2:12" ht="15" customHeight="1">
+      <c r="B61" s="148"/>
+      <c r="C61" s="148"/>
+      <c r="D61" s="138"/>
+      <c r="E61" s="138"/>
+      <c r="F61" s="141"/>
+      <c r="G61" s="142"/>
+      <c r="H61" s="138"/>
+    </row>
+    <row r="62" spans="2:12" ht="15">
+      <c r="B62" s="148"/>
+      <c r="C62" s="148"/>
+      <c r="D62" s="138"/>
+      <c r="E62" s="138"/>
+      <c r="F62" s="143"/>
+      <c r="G62" s="144"/>
+      <c r="H62" s="138"/>
+    </row>
+    <row r="63" spans="2:12" ht="15.75" customHeight="1">
+      <c r="B63" s="148"/>
+      <c r="C63" s="148"/>
       <c r="D63" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="135" t="s">
+      <c r="F63" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="G63" s="136"/>
+      <c r="G63" s="96"/>
       <c r="H63" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:12" ht="15.75" customHeight="1">
       <c r="B64" s="21" t="s">
         <v>89</v>
       </c>
@@ -2589,23 +2440,23 @@
       <c r="E64" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="F64" s="137" t="s">
+      <c r="F64" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="G64" s="138"/>
+      <c r="G64" s="98"/>
       <c r="H64" s="81" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="15">
       <c r="G65" s="14"/>
       <c r="H65" s="63"/>
     </row>
-    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="15">
       <c r="G66" s="14"/>
       <c r="H66" s="13"/>
     </row>
-    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="15.75" customHeight="1">
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
         <v>7</v>
@@ -2620,7 +2471,7 @@
       <c r="G67" s="14"/>
       <c r="H67" s="13"/>
     </row>
-    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="15.75" customHeight="1">
       <c r="A68" s="65"/>
       <c r="B68" s="9"/>
       <c r="C68" s="1" t="s">
@@ -2636,7 +2487,7 @@
       <c r="G68" s="14"/>
       <c r="H68" s="13"/>
     </row>
-    <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="15.75" customHeight="1">
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
         <v>5</v>
@@ -2651,7 +2502,7 @@
       <c r="G69" s="14"/>
       <c r="H69" s="13"/>
     </row>
-    <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="15.75" customHeight="1">
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
         <v>4</v>
@@ -2666,7 +2517,7 @@
       <c r="G70" s="14"/>
       <c r="H70" s="13"/>
     </row>
-    <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="15.75" customHeight="1">
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
         <v>3</v>
@@ -2679,14 +2530,14 @@
       </c>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="15">
       <c r="C72" s="3"/>
       <c r="D72" s="5"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="12"/>
     </row>
-    <row r="73" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="15" customHeight="1">
       <c r="B73" s="9"/>
       <c r="C73" s="75" t="s">
         <v>2</v>
@@ -2702,11 +2553,11 @@
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
     </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B74" s="98" t="s">
+    <row r="74" spans="1:9" ht="15.75">
+      <c r="B74" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="98"/>
+      <c r="C74" s="134"/>
       <c r="D74" s="62" t="s">
         <v>88</v>
       </c>
@@ -2718,7 +2569,7 @@
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
     </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="15.75">
       <c r="B75" s="69"/>
       <c r="C75" s="69"/>
       <c r="D75" s="62"/>
@@ -2728,11 +2579,11 @@
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
     </row>
-    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B76" s="98" t="e" vm="1">
+    <row r="76" spans="1:9" ht="15.75">
+      <c r="B76" s="134" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C76" s="98"/>
+      <c r="C76" s="134"/>
       <c r="D76" s="62"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -2740,9 +2591,9 @@
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
     </row>
-    <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B77" s="98"/>
-      <c r="C77" s="98"/>
+    <row r="77" spans="1:9" ht="15.75">
+      <c r="B77" s="134"/>
+      <c r="C77" s="134"/>
       <c r="D77" s="62"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -2750,9 +2601,9 @@
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
     </row>
-    <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B78" s="98"/>
-      <c r="C78" s="98"/>
+    <row r="78" spans="1:9" ht="15.75">
+      <c r="B78" s="134"/>
+      <c r="C78" s="134"/>
       <c r="D78" s="62"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -2760,9 +2611,9 @@
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
     </row>
-    <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B79" s="98"/>
-      <c r="C79" s="98"/>
+    <row r="79" spans="1:9" ht="15.75">
+      <c r="B79" s="134"/>
+      <c r="C79" s="134"/>
       <c r="D79" s="62"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -2770,9 +2621,9 @@
       <c r="H79" s="9"/>
       <c r="I79" s="9"/>
     </row>
-    <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B80" s="98"/>
-      <c r="C80" s="98"/>
+    <row r="80" spans="1:9" ht="15.75">
+      <c r="B80" s="134"/>
+      <c r="C80" s="134"/>
       <c r="D80" s="62"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -2780,69 +2631,40 @@
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
     </row>
-    <row r="81" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:10" ht="18" customHeight="1">
       <c r="D81" s="64"/>
-      <c r="F81" s="128"/>
+      <c r="F81" s="92"/>
       <c r="G81" s="9"/>
       <c r="H81" s="87"/>
       <c r="I81" s="9"/>
     </row>
-    <row r="82" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="97" t="s">
+    <row r="82" spans="2:10" ht="18" customHeight="1">
+      <c r="B82" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="97"/>
+      <c r="C82" s="133"/>
       <c r="D82" s="88"/>
       <c r="E82" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="F82" s="127"/>
+      <c r="F82" s="91"/>
       <c r="G82" s="85"/>
-      <c r="H82" s="101" t="s">
+      <c r="H82" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="I82" s="101"/>
+      <c r="I82" s="137"/>
       <c r="J82" s="45"/>
     </row>
-    <row r="83" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:10" ht="18" customHeight="1">
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="D1:H3"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="F40:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="D39:D43"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="C39:C44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F22:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="D59:H59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="E60:E62"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="B76:C80"/>
     <mergeCell ref="H49:H50"/>
@@ -2859,9 +2681,38 @@
     <mergeCell ref="I51:I52"/>
     <mergeCell ref="B59:B63"/>
     <mergeCell ref="C59:C63"/>
-    <mergeCell ref="D59:H59"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="D39:D43"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F22:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="D1:H3"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="F40:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>

<commit_message>
cambio en lahoja de diseño de DetermiancionVolGna
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaDeterminacionVolGNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC90E6D8-C659-482A-A782-38AE97C22594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018E7D54-9150-48CD-8454-99E1531C4C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{87F3111E-DF55-4202-AC8E-52B13E902D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="PROPIEDADES" sheetId="6" r:id="rId1"/>
@@ -2189,7 +2189,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="510">
+  <cellXfs count="511">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -3043,9 +3043,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3063,7 +3060,6 @@
     <xf numFmtId="166" fontId="25" fillId="0" borderId="4" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="17" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="17" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="17" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="17" applyBorder="1"/>
@@ -3077,9 +3073,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="25" fillId="0" borderId="10" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="51" fillId="0" borderId="10" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="17" applyFont="1" applyBorder="1"/>
@@ -3132,15 +3125,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="17" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3169,6 +3156,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="17" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="17" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="11" xfId="17" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3220,24 +3209,24 @@
     <xf numFmtId="170" fontId="25" fillId="0" borderId="32" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="10" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3307,161 +3296,197 @@
     <xf numFmtId="0" fontId="40" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="14" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="12" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="5" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="4" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3493,41 +3518,14 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="14" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="12" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="5" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="4" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3541,17 +3539,24 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="9" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="11" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="7" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="7" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="51" fillId="0" borderId="2" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Millares 15" xfId="13" xr:uid="{16186204-111B-4A08-A191-D695A006C21A}"/>
@@ -4885,36 +4890,36 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="15.6">
-      <c r="C3" s="381" t="s">
+      <c r="C3" s="378" t="s">
         <v>100</v>
       </c>
-      <c r="D3" s="381"/>
-      <c r="E3" s="381"/>
+      <c r="D3" s="378"/>
+      <c r="E3" s="378"/>
       <c r="K3" s="90" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="13.8">
-      <c r="A5" s="382" t="s">
+      <c r="A5" s="379" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="383"/>
+      <c r="B5" s="380"/>
       <c r="C5" s="91"/>
       <c r="D5" s="91"/>
       <c r="E5" s="91"/>
       <c r="F5" s="91"/>
-      <c r="I5" s="382" t="s">
+      <c r="I5" s="379" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="383"/>
+      <c r="J5" s="380"/>
       <c r="K5" s="91"/>
       <c r="L5" s="91"/>
       <c r="M5" s="91"/>
       <c r="N5" s="91"/>
     </row>
     <row r="6" spans="1:14" ht="51" customHeight="1">
-      <c r="A6" s="384"/>
-      <c r="B6" s="385"/>
+      <c r="A6" s="381"/>
+      <c r="B6" s="382"/>
       <c r="C6" s="92" t="s">
         <v>103</v>
       </c>
@@ -4927,8 +4932,8 @@
       <c r="F6" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="384"/>
-      <c r="J6" s="385"/>
+      <c r="I6" s="381"/>
+      <c r="J6" s="382"/>
       <c r="K6" s="92" t="s">
         <v>103</v>
       </c>
@@ -4943,8 +4948,8 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="13.8">
-      <c r="A7" s="384"/>
-      <c r="B7" s="385"/>
+      <c r="A7" s="381"/>
+      <c r="B7" s="382"/>
       <c r="C7" s="94" t="s">
         <v>107</v>
       </c>
@@ -4957,8 +4962,8 @@
       <c r="F7" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="384"/>
-      <c r="J7" s="385"/>
+      <c r="I7" s="381"/>
+      <c r="J7" s="382"/>
       <c r="K7" s="94" t="s">
         <v>107</v>
       </c>
@@ -4973,39 +4978,39 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="14.4" thickBot="1">
-      <c r="A8" s="386"/>
-      <c r="B8" s="387"/>
+      <c r="A8" s="383"/>
+      <c r="B8" s="384"/>
       <c r="C8" s="96"/>
       <c r="D8" s="97"/>
       <c r="E8" s="97"/>
       <c r="F8" s="97"/>
       <c r="H8" s="98"/>
-      <c r="I8" s="386"/>
-      <c r="J8" s="387"/>
+      <c r="I8" s="383"/>
+      <c r="J8" s="384"/>
       <c r="K8" s="96"/>
       <c r="L8" s="97"/>
       <c r="M8" s="97"/>
       <c r="N8" s="97"/>
     </row>
     <row r="9" spans="1:14" ht="13.8">
-      <c r="A9" s="392"/>
-      <c r="B9" s="393"/>
+      <c r="A9" s="389"/>
+      <c r="B9" s="390"/>
       <c r="C9" s="99"/>
       <c r="D9" s="100"/>
       <c r="E9" s="100"/>
       <c r="F9" s="101"/>
-      <c r="I9" s="394"/>
-      <c r="J9" s="395"/>
+      <c r="I9" s="391"/>
+      <c r="J9" s="392"/>
       <c r="K9" s="99"/>
       <c r="L9" s="100"/>
       <c r="M9" s="100"/>
       <c r="N9" s="101"/>
     </row>
     <row r="10" spans="1:14" ht="15.6">
-      <c r="A10" s="388" t="s">
+      <c r="A10" s="385" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="389"/>
+      <c r="B10" s="386"/>
       <c r="C10" s="103" t="s">
         <v>250</v>
       </c>
@@ -5018,10 +5023,10 @@
       <c r="F10" s="105" t="s">
         <v>253</v>
       </c>
-      <c r="I10" s="388" t="s">
+      <c r="I10" s="385" t="s">
         <v>249</v>
       </c>
-      <c r="J10" s="389"/>
+      <c r="J10" s="386"/>
       <c r="K10" s="103" t="s">
         <v>250</v>
       </c>
@@ -5036,18 +5041,18 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.6">
-      <c r="A11" s="390"/>
-      <c r="B11" s="391"/>
-      <c r="C11" s="374"/>
-      <c r="D11" s="375"/>
-      <c r="E11" s="375"/>
-      <c r="F11" s="376"/>
-      <c r="I11" s="390"/>
-      <c r="J11" s="391"/>
-      <c r="K11" s="374"/>
-      <c r="L11" s="375"/>
-      <c r="M11" s="375"/>
-      <c r="N11" s="376"/>
+      <c r="A11" s="387"/>
+      <c r="B11" s="388"/>
+      <c r="C11" s="369"/>
+      <c r="D11" s="370"/>
+      <c r="E11" s="370"/>
+      <c r="F11" s="371"/>
+      <c r="I11" s="387"/>
+      <c r="J11" s="388"/>
+      <c r="K11" s="369"/>
+      <c r="L11" s="370"/>
+      <c r="M11" s="370"/>
+      <c r="N11" s="371"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5187,10 +5192,10 @@
       <c r="H10" s="124"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="396" t="s">
+      <c r="A11" s="393" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="397"/>
+      <c r="B11" s="394"/>
       <c r="C11" s="129" t="s">
         <v>254</v>
       </c>
@@ -5199,8 +5204,8 @@
       <c r="H11" s="124"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="396"/>
-      <c r="B12" s="397"/>
+      <c r="A12" s="393"/>
+      <c r="B12" s="394"/>
       <c r="C12" s="132"/>
       <c r="D12" s="130"/>
       <c r="H12" s="124"/>
@@ -5567,7 +5572,7 @@
     </row>
     <row r="18" spans="1:10" s="174" customFormat="1">
       <c r="A18" s="143"/>
-      <c r="B18" s="400" t="s">
+      <c r="B18" s="395" t="s">
         <v>137</v>
       </c>
       <c r="C18" s="156" t="s">
@@ -5580,7 +5585,7 @@
     </row>
     <row r="19" spans="1:10" s="174" customFormat="1" ht="13.8" thickBot="1">
       <c r="A19" s="184"/>
-      <c r="B19" s="401"/>
+      <c r="B19" s="396"/>
       <c r="C19" s="185" t="s">
         <v>132</v>
       </c>
@@ -5632,7 +5637,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="143"/>
-      <c r="B24" s="400" t="s">
+      <c r="B24" s="395" t="s">
         <v>137</v>
       </c>
       <c r="C24" s="156" t="s">
@@ -5642,7 +5647,7 @@
     </row>
     <row r="25" spans="1:10" ht="13.8" thickBot="1">
       <c r="A25" s="143"/>
-      <c r="B25" s="401"/>
+      <c r="B25" s="396"/>
       <c r="C25" s="185" t="s">
         <v>143</v>
       </c>
@@ -5704,7 +5709,7 @@
     </row>
     <row r="31" spans="1:10" s="200" customFormat="1">
       <c r="A31" s="196"/>
-      <c r="B31" s="402" t="s">
+      <c r="B31" s="397" t="s">
         <v>148</v>
       </c>
       <c r="C31" s="201" t="s">
@@ -5717,7 +5722,7 @@
     </row>
     <row r="32" spans="1:10" s="200" customFormat="1" ht="13.8" thickBot="1">
       <c r="A32" s="196"/>
-      <c r="B32" s="403"/>
+      <c r="B32" s="398"/>
       <c r="C32" s="203" t="s">
         <v>132</v>
       </c>
@@ -5834,166 +5839,166 @@
       <c r="D51" s="211"/>
       <c r="E51" s="211"/>
       <c r="F51" s="211"/>
-      <c r="G51" s="398"/>
-      <c r="H51" s="398"/>
-      <c r="I51" s="398"/>
-      <c r="J51" s="398"/>
-      <c r="K51" s="398"/>
-      <c r="L51" s="398"/>
-      <c r="M51" s="398"/>
-      <c r="N51" s="398"/>
-      <c r="O51" s="398"/>
-      <c r="P51" s="398"/>
-      <c r="Q51" s="398"/>
-      <c r="R51" s="398"/>
-      <c r="S51" s="398"/>
-      <c r="T51" s="398"/>
-      <c r="U51" s="398"/>
-      <c r="V51" s="398"/>
-      <c r="W51" s="398"/>
-      <c r="X51" s="398"/>
-      <c r="Y51" s="398"/>
-      <c r="Z51" s="398"/>
-      <c r="AA51" s="398"/>
-      <c r="AB51" s="398"/>
-      <c r="AC51" s="398"/>
-      <c r="AD51" s="398"/>
-      <c r="AE51" s="398"/>
-      <c r="AF51" s="398"/>
-      <c r="AG51" s="398"/>
-      <c r="AH51" s="398"/>
-      <c r="AI51" s="398"/>
-      <c r="AJ51" s="398"/>
-      <c r="AK51" s="398"/>
-      <c r="AL51" s="398"/>
-      <c r="AM51" s="398"/>
-      <c r="AN51" s="398"/>
-      <c r="AO51" s="398"/>
-      <c r="AP51" s="398"/>
-      <c r="AQ51" s="398"/>
-      <c r="AR51" s="398"/>
-      <c r="AS51" s="398"/>
-      <c r="AT51" s="398"/>
-      <c r="AU51" s="398"/>
-      <c r="AV51" s="398"/>
-      <c r="AW51" s="398"/>
-      <c r="AX51" s="398"/>
-      <c r="AY51" s="398"/>
-      <c r="AZ51" s="398"/>
-      <c r="BA51" s="398"/>
-      <c r="BB51" s="398"/>
-      <c r="BC51" s="398"/>
-      <c r="BD51" s="398"/>
-      <c r="BE51" s="398"/>
-      <c r="BF51" s="398"/>
-      <c r="BG51" s="398"/>
-      <c r="BH51" s="398"/>
-      <c r="BI51" s="398"/>
-      <c r="BJ51" s="398"/>
-      <c r="BK51" s="398"/>
-      <c r="BL51" s="398"/>
-      <c r="BM51" s="398"/>
-      <c r="BN51" s="398"/>
-      <c r="BO51" s="398"/>
-      <c r="BP51" s="398"/>
-      <c r="BQ51" s="398"/>
-      <c r="BR51" s="398"/>
-      <c r="BS51" s="398"/>
-      <c r="BT51" s="398"/>
-      <c r="BU51" s="398"/>
-      <c r="BV51" s="398"/>
-      <c r="BW51" s="398"/>
-      <c r="BX51" s="398"/>
-      <c r="BY51" s="398"/>
-      <c r="BZ51" s="398"/>
-      <c r="CA51" s="398"/>
-      <c r="CB51" s="398"/>
-      <c r="CC51" s="398"/>
-      <c r="CD51" s="398"/>
-      <c r="CE51" s="398"/>
-      <c r="CF51" s="398"/>
-      <c r="CG51" s="398"/>
-      <c r="CH51" s="398"/>
-      <c r="CI51" s="398"/>
-      <c r="CJ51" s="398"/>
-      <c r="CK51" s="398"/>
-      <c r="CL51" s="398"/>
-      <c r="CM51" s="398"/>
-      <c r="CN51" s="398"/>
-      <c r="CO51" s="398"/>
-      <c r="CP51" s="398"/>
-      <c r="CQ51" s="398"/>
-      <c r="CR51" s="398"/>
-      <c r="CS51" s="398"/>
-      <c r="CT51" s="398"/>
-      <c r="CU51" s="398"/>
-      <c r="CV51" s="398"/>
-      <c r="CW51" s="398"/>
-      <c r="CX51" s="398"/>
-      <c r="CY51" s="398"/>
-      <c r="CZ51" s="398"/>
-      <c r="DA51" s="398"/>
-      <c r="DB51" s="398"/>
-      <c r="DC51" s="398"/>
-      <c r="DD51" s="398"/>
-      <c r="DE51" s="398"/>
-      <c r="DF51" s="398"/>
-      <c r="DG51" s="398"/>
-      <c r="DH51" s="398"/>
-      <c r="DI51" s="398"/>
-      <c r="DJ51" s="398"/>
-      <c r="DK51" s="398"/>
-      <c r="DL51" s="398"/>
-      <c r="DM51" s="398"/>
-      <c r="DN51" s="398"/>
-      <c r="DO51" s="398"/>
-      <c r="DP51" s="398"/>
-      <c r="DQ51" s="398"/>
-      <c r="DR51" s="398"/>
-      <c r="DS51" s="398"/>
-      <c r="DT51" s="398"/>
-      <c r="DU51" s="398"/>
-      <c r="DV51" s="398"/>
-      <c r="DW51" s="398"/>
-      <c r="DX51" s="398"/>
-      <c r="DY51" s="398"/>
-      <c r="DZ51" s="398"/>
-      <c r="EA51" s="398"/>
-      <c r="EB51" s="398"/>
-      <c r="EC51" s="398"/>
-      <c r="ED51" s="398"/>
-      <c r="EE51" s="398"/>
-      <c r="EF51" s="398"/>
-      <c r="EG51" s="398"/>
-      <c r="EH51" s="398"/>
-      <c r="EI51" s="398"/>
-      <c r="EJ51" s="398"/>
-      <c r="EK51" s="398"/>
-      <c r="EL51" s="398"/>
-      <c r="EM51" s="398"/>
-      <c r="EN51" s="398"/>
-      <c r="EO51" s="398"/>
-      <c r="EP51" s="398"/>
-      <c r="EQ51" s="398"/>
-      <c r="ER51" s="398"/>
-      <c r="ES51" s="398"/>
-      <c r="ET51" s="398"/>
-      <c r="EU51" s="398"/>
-      <c r="EV51" s="398"/>
-      <c r="EW51" s="398"/>
-      <c r="EX51" s="398"/>
-      <c r="EY51" s="398"/>
-      <c r="EZ51" s="398"/>
-      <c r="FA51" s="398"/>
-      <c r="FB51" s="398"/>
-      <c r="FC51" s="398"/>
-      <c r="FD51" s="398"/>
-      <c r="FE51" s="398"/>
-      <c r="FF51" s="398"/>
-      <c r="FG51" s="398"/>
-      <c r="FH51" s="398"/>
-      <c r="FI51" s="398"/>
-      <c r="FJ51" s="398"/>
+      <c r="G51" s="399"/>
+      <c r="H51" s="399"/>
+      <c r="I51" s="399"/>
+      <c r="J51" s="399"/>
+      <c r="K51" s="399"/>
+      <c r="L51" s="399"/>
+      <c r="M51" s="399"/>
+      <c r="N51" s="399"/>
+      <c r="O51" s="399"/>
+      <c r="P51" s="399"/>
+      <c r="Q51" s="399"/>
+      <c r="R51" s="399"/>
+      <c r="S51" s="399"/>
+      <c r="T51" s="399"/>
+      <c r="U51" s="399"/>
+      <c r="V51" s="399"/>
+      <c r="W51" s="399"/>
+      <c r="X51" s="399"/>
+      <c r="Y51" s="399"/>
+      <c r="Z51" s="399"/>
+      <c r="AA51" s="399"/>
+      <c r="AB51" s="399"/>
+      <c r="AC51" s="399"/>
+      <c r="AD51" s="399"/>
+      <c r="AE51" s="399"/>
+      <c r="AF51" s="399"/>
+      <c r="AG51" s="399"/>
+      <c r="AH51" s="399"/>
+      <c r="AI51" s="399"/>
+      <c r="AJ51" s="399"/>
+      <c r="AK51" s="399"/>
+      <c r="AL51" s="399"/>
+      <c r="AM51" s="399"/>
+      <c r="AN51" s="399"/>
+      <c r="AO51" s="399"/>
+      <c r="AP51" s="399"/>
+      <c r="AQ51" s="399"/>
+      <c r="AR51" s="399"/>
+      <c r="AS51" s="399"/>
+      <c r="AT51" s="399"/>
+      <c r="AU51" s="399"/>
+      <c r="AV51" s="399"/>
+      <c r="AW51" s="399"/>
+      <c r="AX51" s="399"/>
+      <c r="AY51" s="399"/>
+      <c r="AZ51" s="399"/>
+      <c r="BA51" s="399"/>
+      <c r="BB51" s="399"/>
+      <c r="BC51" s="399"/>
+      <c r="BD51" s="399"/>
+      <c r="BE51" s="399"/>
+      <c r="BF51" s="399"/>
+      <c r="BG51" s="399"/>
+      <c r="BH51" s="399"/>
+      <c r="BI51" s="399"/>
+      <c r="BJ51" s="399"/>
+      <c r="BK51" s="399"/>
+      <c r="BL51" s="399"/>
+      <c r="BM51" s="399"/>
+      <c r="BN51" s="399"/>
+      <c r="BO51" s="399"/>
+      <c r="BP51" s="399"/>
+      <c r="BQ51" s="399"/>
+      <c r="BR51" s="399"/>
+      <c r="BS51" s="399"/>
+      <c r="BT51" s="399"/>
+      <c r="BU51" s="399"/>
+      <c r="BV51" s="399"/>
+      <c r="BW51" s="399"/>
+      <c r="BX51" s="399"/>
+      <c r="BY51" s="399"/>
+      <c r="BZ51" s="399"/>
+      <c r="CA51" s="399"/>
+      <c r="CB51" s="399"/>
+      <c r="CC51" s="399"/>
+      <c r="CD51" s="399"/>
+      <c r="CE51" s="399"/>
+      <c r="CF51" s="399"/>
+      <c r="CG51" s="399"/>
+      <c r="CH51" s="399"/>
+      <c r="CI51" s="399"/>
+      <c r="CJ51" s="399"/>
+      <c r="CK51" s="399"/>
+      <c r="CL51" s="399"/>
+      <c r="CM51" s="399"/>
+      <c r="CN51" s="399"/>
+      <c r="CO51" s="399"/>
+      <c r="CP51" s="399"/>
+      <c r="CQ51" s="399"/>
+      <c r="CR51" s="399"/>
+      <c r="CS51" s="399"/>
+      <c r="CT51" s="399"/>
+      <c r="CU51" s="399"/>
+      <c r="CV51" s="399"/>
+      <c r="CW51" s="399"/>
+      <c r="CX51" s="399"/>
+      <c r="CY51" s="399"/>
+      <c r="CZ51" s="399"/>
+      <c r="DA51" s="399"/>
+      <c r="DB51" s="399"/>
+      <c r="DC51" s="399"/>
+      <c r="DD51" s="399"/>
+      <c r="DE51" s="399"/>
+      <c r="DF51" s="399"/>
+      <c r="DG51" s="399"/>
+      <c r="DH51" s="399"/>
+      <c r="DI51" s="399"/>
+      <c r="DJ51" s="399"/>
+      <c r="DK51" s="399"/>
+      <c r="DL51" s="399"/>
+      <c r="DM51" s="399"/>
+      <c r="DN51" s="399"/>
+      <c r="DO51" s="399"/>
+      <c r="DP51" s="399"/>
+      <c r="DQ51" s="399"/>
+      <c r="DR51" s="399"/>
+      <c r="DS51" s="399"/>
+      <c r="DT51" s="399"/>
+      <c r="DU51" s="399"/>
+      <c r="DV51" s="399"/>
+      <c r="DW51" s="399"/>
+      <c r="DX51" s="399"/>
+      <c r="DY51" s="399"/>
+      <c r="DZ51" s="399"/>
+      <c r="EA51" s="399"/>
+      <c r="EB51" s="399"/>
+      <c r="EC51" s="399"/>
+      <c r="ED51" s="399"/>
+      <c r="EE51" s="399"/>
+      <c r="EF51" s="399"/>
+      <c r="EG51" s="399"/>
+      <c r="EH51" s="399"/>
+      <c r="EI51" s="399"/>
+      <c r="EJ51" s="399"/>
+      <c r="EK51" s="399"/>
+      <c r="EL51" s="399"/>
+      <c r="EM51" s="399"/>
+      <c r="EN51" s="399"/>
+      <c r="EO51" s="399"/>
+      <c r="EP51" s="399"/>
+      <c r="EQ51" s="399"/>
+      <c r="ER51" s="399"/>
+      <c r="ES51" s="399"/>
+      <c r="ET51" s="399"/>
+      <c r="EU51" s="399"/>
+      <c r="EV51" s="399"/>
+      <c r="EW51" s="399"/>
+      <c r="EX51" s="399"/>
+      <c r="EY51" s="399"/>
+      <c r="EZ51" s="399"/>
+      <c r="FA51" s="399"/>
+      <c r="FB51" s="399"/>
+      <c r="FC51" s="399"/>
+      <c r="FD51" s="399"/>
+      <c r="FE51" s="399"/>
+      <c r="FF51" s="399"/>
+      <c r="FG51" s="399"/>
+      <c r="FH51" s="399"/>
+      <c r="FI51" s="399"/>
+      <c r="FJ51" s="399"/>
     </row>
     <row r="52" spans="1:166" ht="18" customHeight="1">
       <c r="A52" s="211"/>
@@ -6002,172 +6007,172 @@
       <c r="D52" s="211"/>
       <c r="E52" s="211"/>
       <c r="F52" s="211"/>
-      <c r="G52" s="398"/>
-      <c r="H52" s="398"/>
-      <c r="I52" s="398"/>
-      <c r="J52" s="398"/>
-      <c r="K52" s="398"/>
-      <c r="L52" s="398"/>
-      <c r="M52" s="398"/>
-      <c r="N52" s="398"/>
-      <c r="O52" s="398"/>
-      <c r="P52" s="398"/>
-      <c r="Q52" s="398"/>
-      <c r="R52" s="398"/>
-      <c r="S52" s="398"/>
-      <c r="T52" s="398"/>
-      <c r="U52" s="398"/>
-      <c r="V52" s="398"/>
-      <c r="W52" s="398"/>
-      <c r="X52" s="398"/>
-      <c r="Y52" s="398"/>
-      <c r="Z52" s="398"/>
-      <c r="AA52" s="398"/>
-      <c r="AB52" s="398"/>
-      <c r="AC52" s="398"/>
-      <c r="AD52" s="398"/>
-      <c r="AE52" s="398"/>
-      <c r="AF52" s="398"/>
-      <c r="AG52" s="398"/>
-      <c r="AH52" s="398"/>
-      <c r="AI52" s="398"/>
-      <c r="AJ52" s="398"/>
-      <c r="AK52" s="398"/>
-      <c r="AL52" s="398"/>
-      <c r="AM52" s="398"/>
-      <c r="AN52" s="398"/>
-      <c r="AO52" s="398"/>
-      <c r="AP52" s="398"/>
-      <c r="AQ52" s="398"/>
-      <c r="AR52" s="398"/>
-      <c r="AS52" s="398"/>
-      <c r="AT52" s="398"/>
-      <c r="AU52" s="398"/>
-      <c r="AV52" s="398"/>
-      <c r="AW52" s="398"/>
-      <c r="AX52" s="398"/>
-      <c r="AY52" s="398"/>
-      <c r="AZ52" s="398"/>
-      <c r="BA52" s="398"/>
-      <c r="BB52" s="398"/>
-      <c r="BC52" s="398"/>
-      <c r="BD52" s="398"/>
-      <c r="BE52" s="398"/>
-      <c r="BF52" s="398"/>
-      <c r="BG52" s="398"/>
-      <c r="BH52" s="398"/>
-      <c r="BI52" s="398"/>
-      <c r="BJ52" s="398"/>
-      <c r="BK52" s="398"/>
-      <c r="BL52" s="398"/>
-      <c r="BM52" s="398"/>
-      <c r="BN52" s="398"/>
-      <c r="BO52" s="398"/>
-      <c r="BP52" s="398"/>
-      <c r="BQ52" s="398"/>
-      <c r="BR52" s="398"/>
-      <c r="BS52" s="398"/>
-      <c r="BT52" s="398"/>
-      <c r="BU52" s="398"/>
-      <c r="BV52" s="398"/>
-      <c r="BW52" s="398"/>
-      <c r="BX52" s="398"/>
-      <c r="BY52" s="398"/>
-      <c r="BZ52" s="398"/>
-      <c r="CA52" s="398"/>
-      <c r="CB52" s="398"/>
-      <c r="CC52" s="398"/>
-      <c r="CD52" s="398"/>
-      <c r="CE52" s="398"/>
-      <c r="CF52" s="398"/>
-      <c r="CG52" s="398"/>
-      <c r="CH52" s="398"/>
-      <c r="CI52" s="398"/>
-      <c r="CJ52" s="398"/>
-      <c r="CK52" s="398"/>
-      <c r="CL52" s="398"/>
-      <c r="CM52" s="398"/>
-      <c r="CN52" s="398"/>
-      <c r="CO52" s="398"/>
-      <c r="CP52" s="398"/>
-      <c r="CQ52" s="398"/>
-      <c r="CR52" s="398"/>
-      <c r="CS52" s="398"/>
-      <c r="CT52" s="398"/>
-      <c r="CU52" s="398"/>
-      <c r="CV52" s="398"/>
-      <c r="CW52" s="398"/>
-      <c r="CX52" s="398"/>
-      <c r="CY52" s="398"/>
-      <c r="CZ52" s="398"/>
-      <c r="DA52" s="398"/>
-      <c r="DB52" s="398"/>
-      <c r="DC52" s="398"/>
-      <c r="DD52" s="398"/>
-      <c r="DE52" s="398"/>
-      <c r="DF52" s="398"/>
-      <c r="DG52" s="398"/>
-      <c r="DH52" s="398"/>
-      <c r="DI52" s="398"/>
-      <c r="DJ52" s="398"/>
-      <c r="DK52" s="398"/>
-      <c r="DL52" s="398"/>
-      <c r="DM52" s="398"/>
-      <c r="DN52" s="398"/>
-      <c r="DO52" s="398"/>
-      <c r="DP52" s="398"/>
-      <c r="DQ52" s="398"/>
-      <c r="DR52" s="398"/>
-      <c r="DS52" s="398"/>
-      <c r="DT52" s="398"/>
-      <c r="DU52" s="398"/>
-      <c r="DV52" s="398"/>
-      <c r="DW52" s="398"/>
-      <c r="DX52" s="398"/>
-      <c r="DY52" s="398"/>
-      <c r="DZ52" s="398"/>
-      <c r="EA52" s="398"/>
-      <c r="EB52" s="398"/>
-      <c r="EC52" s="398"/>
-      <c r="ED52" s="398"/>
-      <c r="EE52" s="398"/>
-      <c r="EF52" s="398"/>
-      <c r="EG52" s="398"/>
-      <c r="EH52" s="398"/>
-      <c r="EI52" s="398"/>
-      <c r="EJ52" s="398"/>
-      <c r="EK52" s="398"/>
-      <c r="EL52" s="398"/>
-      <c r="EM52" s="398"/>
-      <c r="EN52" s="398"/>
-      <c r="EO52" s="398"/>
-      <c r="EP52" s="398"/>
-      <c r="EQ52" s="398"/>
-      <c r="ER52" s="398"/>
-      <c r="ES52" s="398"/>
-      <c r="ET52" s="398"/>
-      <c r="EU52" s="398"/>
-      <c r="EV52" s="398"/>
-      <c r="EW52" s="398"/>
-      <c r="EX52" s="398"/>
-      <c r="EY52" s="398"/>
-      <c r="EZ52" s="398"/>
-      <c r="FA52" s="398"/>
-      <c r="FB52" s="398"/>
-      <c r="FC52" s="398"/>
-      <c r="FD52" s="398"/>
-      <c r="FE52" s="398"/>
-      <c r="FF52" s="398"/>
-      <c r="FG52" s="398"/>
-      <c r="FH52" s="398"/>
-      <c r="FI52" s="398"/>
-      <c r="FJ52" s="398"/>
+      <c r="G52" s="399"/>
+      <c r="H52" s="399"/>
+      <c r="I52" s="399"/>
+      <c r="J52" s="399"/>
+      <c r="K52" s="399"/>
+      <c r="L52" s="399"/>
+      <c r="M52" s="399"/>
+      <c r="N52" s="399"/>
+      <c r="O52" s="399"/>
+      <c r="P52" s="399"/>
+      <c r="Q52" s="399"/>
+      <c r="R52" s="399"/>
+      <c r="S52" s="399"/>
+      <c r="T52" s="399"/>
+      <c r="U52" s="399"/>
+      <c r="V52" s="399"/>
+      <c r="W52" s="399"/>
+      <c r="X52" s="399"/>
+      <c r="Y52" s="399"/>
+      <c r="Z52" s="399"/>
+      <c r="AA52" s="399"/>
+      <c r="AB52" s="399"/>
+      <c r="AC52" s="399"/>
+      <c r="AD52" s="399"/>
+      <c r="AE52" s="399"/>
+      <c r="AF52" s="399"/>
+      <c r="AG52" s="399"/>
+      <c r="AH52" s="399"/>
+      <c r="AI52" s="399"/>
+      <c r="AJ52" s="399"/>
+      <c r="AK52" s="399"/>
+      <c r="AL52" s="399"/>
+      <c r="AM52" s="399"/>
+      <c r="AN52" s="399"/>
+      <c r="AO52" s="399"/>
+      <c r="AP52" s="399"/>
+      <c r="AQ52" s="399"/>
+      <c r="AR52" s="399"/>
+      <c r="AS52" s="399"/>
+      <c r="AT52" s="399"/>
+      <c r="AU52" s="399"/>
+      <c r="AV52" s="399"/>
+      <c r="AW52" s="399"/>
+      <c r="AX52" s="399"/>
+      <c r="AY52" s="399"/>
+      <c r="AZ52" s="399"/>
+      <c r="BA52" s="399"/>
+      <c r="BB52" s="399"/>
+      <c r="BC52" s="399"/>
+      <c r="BD52" s="399"/>
+      <c r="BE52" s="399"/>
+      <c r="BF52" s="399"/>
+      <c r="BG52" s="399"/>
+      <c r="BH52" s="399"/>
+      <c r="BI52" s="399"/>
+      <c r="BJ52" s="399"/>
+      <c r="BK52" s="399"/>
+      <c r="BL52" s="399"/>
+      <c r="BM52" s="399"/>
+      <c r="BN52" s="399"/>
+      <c r="BO52" s="399"/>
+      <c r="BP52" s="399"/>
+      <c r="BQ52" s="399"/>
+      <c r="BR52" s="399"/>
+      <c r="BS52" s="399"/>
+      <c r="BT52" s="399"/>
+      <c r="BU52" s="399"/>
+      <c r="BV52" s="399"/>
+      <c r="BW52" s="399"/>
+      <c r="BX52" s="399"/>
+      <c r="BY52" s="399"/>
+      <c r="BZ52" s="399"/>
+      <c r="CA52" s="399"/>
+      <c r="CB52" s="399"/>
+      <c r="CC52" s="399"/>
+      <c r="CD52" s="399"/>
+      <c r="CE52" s="399"/>
+      <c r="CF52" s="399"/>
+      <c r="CG52" s="399"/>
+      <c r="CH52" s="399"/>
+      <c r="CI52" s="399"/>
+      <c r="CJ52" s="399"/>
+      <c r="CK52" s="399"/>
+      <c r="CL52" s="399"/>
+      <c r="CM52" s="399"/>
+      <c r="CN52" s="399"/>
+      <c r="CO52" s="399"/>
+      <c r="CP52" s="399"/>
+      <c r="CQ52" s="399"/>
+      <c r="CR52" s="399"/>
+      <c r="CS52" s="399"/>
+      <c r="CT52" s="399"/>
+      <c r="CU52" s="399"/>
+      <c r="CV52" s="399"/>
+      <c r="CW52" s="399"/>
+      <c r="CX52" s="399"/>
+      <c r="CY52" s="399"/>
+      <c r="CZ52" s="399"/>
+      <c r="DA52" s="399"/>
+      <c r="DB52" s="399"/>
+      <c r="DC52" s="399"/>
+      <c r="DD52" s="399"/>
+      <c r="DE52" s="399"/>
+      <c r="DF52" s="399"/>
+      <c r="DG52" s="399"/>
+      <c r="DH52" s="399"/>
+      <c r="DI52" s="399"/>
+      <c r="DJ52" s="399"/>
+      <c r="DK52" s="399"/>
+      <c r="DL52" s="399"/>
+      <c r="DM52" s="399"/>
+      <c r="DN52" s="399"/>
+      <c r="DO52" s="399"/>
+      <c r="DP52" s="399"/>
+      <c r="DQ52" s="399"/>
+      <c r="DR52" s="399"/>
+      <c r="DS52" s="399"/>
+      <c r="DT52" s="399"/>
+      <c r="DU52" s="399"/>
+      <c r="DV52" s="399"/>
+      <c r="DW52" s="399"/>
+      <c r="DX52" s="399"/>
+      <c r="DY52" s="399"/>
+      <c r="DZ52" s="399"/>
+      <c r="EA52" s="399"/>
+      <c r="EB52" s="399"/>
+      <c r="EC52" s="399"/>
+      <c r="ED52" s="399"/>
+      <c r="EE52" s="399"/>
+      <c r="EF52" s="399"/>
+      <c r="EG52" s="399"/>
+      <c r="EH52" s="399"/>
+      <c r="EI52" s="399"/>
+      <c r="EJ52" s="399"/>
+      <c r="EK52" s="399"/>
+      <c r="EL52" s="399"/>
+      <c r="EM52" s="399"/>
+      <c r="EN52" s="399"/>
+      <c r="EO52" s="399"/>
+      <c r="EP52" s="399"/>
+      <c r="EQ52" s="399"/>
+      <c r="ER52" s="399"/>
+      <c r="ES52" s="399"/>
+      <c r="ET52" s="399"/>
+      <c r="EU52" s="399"/>
+      <c r="EV52" s="399"/>
+      <c r="EW52" s="399"/>
+      <c r="EX52" s="399"/>
+      <c r="EY52" s="399"/>
+      <c r="EZ52" s="399"/>
+      <c r="FA52" s="399"/>
+      <c r="FB52" s="399"/>
+      <c r="FC52" s="399"/>
+      <c r="FD52" s="399"/>
+      <c r="FE52" s="399"/>
+      <c r="FF52" s="399"/>
+      <c r="FG52" s="399"/>
+      <c r="FH52" s="399"/>
+      <c r="FI52" s="399"/>
+      <c r="FJ52" s="399"/>
     </row>
     <row r="53" spans="1:166" ht="19.5" customHeight="1">
-      <c r="A53" s="399"/>
-      <c r="B53" s="399"/>
-      <c r="C53" s="399"/>
-      <c r="D53" s="399"/>
+      <c r="A53" s="400"/>
+      <c r="B53" s="400"/>
+      <c r="C53" s="400"/>
+      <c r="D53" s="400"/>
       <c r="E53" s="212"/>
       <c r="F53" s="212"/>
     </row>
@@ -6190,11 +6195,6 @@
     <row r="56" spans="1:166" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="I51:AD51"/>
     <mergeCell ref="CY52:DV52"/>
     <mergeCell ref="DW52:ET52"/>
     <mergeCell ref="EU52:FJ52"/>
@@ -6210,6 +6210,11 @@
     <mergeCell ref="BC52:BZ52"/>
     <mergeCell ref="CA52:CX52"/>
     <mergeCell ref="AE51:BB51"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:AD51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6247,10 +6252,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="26.25" customHeight="1">
-      <c r="A1" s="406" t="s">
+      <c r="A1" s="403" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="407"/>
+      <c r="B1" s="404"/>
       <c r="C1" s="213"/>
       <c r="D1" s="213"/>
       <c r="E1" s="213"/>
@@ -6259,36 +6264,36 @@
       <c r="H1" s="213"/>
       <c r="I1" s="213"/>
       <c r="J1" s="213"/>
-      <c r="K1" s="408" t="s">
+      <c r="K1" s="405" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="408"/>
-      <c r="M1" s="408"/>
-      <c r="N1" s="408"/>
+      <c r="L1" s="405"/>
+      <c r="M1" s="405"/>
+      <c r="N1" s="405"/>
     </row>
     <row r="2" spans="1:28" ht="58.5" customHeight="1">
       <c r="A2" s="215"/>
       <c r="B2" s="216"/>
-      <c r="C2" s="409" t="s">
+      <c r="C2" s="406" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="410"/>
-      <c r="E2" s="410"/>
-      <c r="F2" s="410"/>
-      <c r="G2" s="410"/>
-      <c r="H2" s="410"/>
-      <c r="I2" s="410"/>
+      <c r="D2" s="407"/>
+      <c r="E2" s="407"/>
+      <c r="F2" s="407"/>
+      <c r="G2" s="407"/>
+      <c r="H2" s="407"/>
+      <c r="I2" s="407"/>
       <c r="J2" s="217"/>
-      <c r="K2" s="408"/>
-      <c r="L2" s="408"/>
-      <c r="M2" s="408"/>
-      <c r="N2" s="408"/>
+      <c r="K2" s="405"/>
+      <c r="L2" s="405"/>
+      <c r="M2" s="405"/>
+      <c r="N2" s="405"/>
     </row>
     <row r="3" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A3" s="411" t="s">
+      <c r="A3" s="408" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="412"/>
+      <c r="B3" s="409"/>
       <c r="C3" s="107"/>
       <c r="D3" s="107"/>
       <c r="E3" s="107"/>
@@ -6347,7 +6352,7 @@
     <row r="6" spans="1:28" ht="14.4">
       <c r="A6" s="221"/>
       <c r="B6" s="102"/>
-      <c r="C6" s="378"/>
+      <c r="C6" s="373"/>
       <c r="D6" s="102"/>
       <c r="E6" s="102"/>
       <c r="F6" s="102"/>
@@ -6598,30 +6603,30 @@
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1">
       <c r="A16" s="224"/>
-      <c r="B16" s="413" t="s">
+      <c r="B16" s="410" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="413"/>
+      <c r="C16" s="410"/>
       <c r="D16" s="252" t="s">
         <v>172</v>
       </c>
-      <c r="E16" s="414" t="s">
+      <c r="E16" s="411" t="s">
         <v>173</v>
       </c>
-      <c r="F16" s="415"/>
-      <c r="G16" s="418" t="s">
+      <c r="F16" s="412"/>
+      <c r="G16" s="415" t="s">
         <v>174</v>
       </c>
-      <c r="H16" s="421" t="s">
+      <c r="H16" s="418" t="s">
         <v>175</v>
       </c>
-      <c r="I16" s="422"/>
-      <c r="J16" s="421" t="s">
+      <c r="I16" s="419"/>
+      <c r="J16" s="418" t="s">
         <v>176</v>
       </c>
-      <c r="K16" s="425"/>
-      <c r="L16" s="425"/>
-      <c r="M16" s="422"/>
+      <c r="K16" s="422"/>
+      <c r="L16" s="422"/>
+      <c r="M16" s="419"/>
       <c r="N16" s="216"/>
       <c r="Q16" s="133"/>
       <c r="R16" s="133"/>
@@ -6638,18 +6643,18 @@
     </row>
     <row r="17" spans="1:28" ht="43.5" customHeight="1">
       <c r="A17" s="224"/>
-      <c r="B17" s="413"/>
-      <c r="C17" s="413"/>
+      <c r="B17" s="410"/>
+      <c r="C17" s="410"/>
       <c r="D17" s="254"/>
-      <c r="E17" s="416"/>
-      <c r="F17" s="417"/>
-      <c r="G17" s="419"/>
-      <c r="H17" s="423"/>
-      <c r="I17" s="424"/>
-      <c r="J17" s="423"/>
-      <c r="K17" s="426"/>
-      <c r="L17" s="426"/>
-      <c r="M17" s="424"/>
+      <c r="E17" s="413"/>
+      <c r="F17" s="414"/>
+      <c r="G17" s="416"/>
+      <c r="H17" s="420"/>
+      <c r="I17" s="421"/>
+      <c r="J17" s="420"/>
+      <c r="K17" s="423"/>
+      <c r="L17" s="423"/>
+      <c r="M17" s="421"/>
       <c r="N17" s="216"/>
       <c r="Q17" s="133"/>
       <c r="R17" s="133"/>
@@ -6666,8 +6671,8 @@
     </row>
     <row r="18" spans="1:28" ht="47.25" customHeight="1">
       <c r="A18" s="224"/>
-      <c r="B18" s="413"/>
-      <c r="C18" s="413"/>
+      <c r="B18" s="410"/>
+      <c r="C18" s="410"/>
       <c r="D18" s="255" t="s">
         <v>177</v>
       </c>
@@ -6677,21 +6682,21 @@
       <c r="F18" s="257" t="s">
         <v>179</v>
       </c>
-      <c r="G18" s="419"/>
+      <c r="G18" s="416"/>
       <c r="H18" s="253" t="s">
         <v>138</v>
       </c>
       <c r="I18" s="258" t="s">
         <v>180</v>
       </c>
-      <c r="J18" s="404" t="s">
+      <c r="J18" s="401" t="s">
         <v>144</v>
       </c>
-      <c r="K18" s="405"/>
-      <c r="L18" s="404" t="s">
+      <c r="K18" s="402"/>
+      <c r="L18" s="401" t="s">
         <v>181</v>
       </c>
-      <c r="M18" s="405"/>
+      <c r="M18" s="402"/>
       <c r="N18" s="216"/>
       <c r="Q18" s="133"/>
       <c r="R18" s="133"/>
@@ -6708,14 +6713,14 @@
     </row>
     <row r="19" spans="1:28" ht="24" customHeight="1">
       <c r="A19" s="224"/>
-      <c r="B19" s="413"/>
-      <c r="C19" s="413"/>
+      <c r="B19" s="410"/>
+      <c r="C19" s="410"/>
       <c r="D19" s="259"/>
       <c r="E19" s="260" t="s">
         <v>182</v>
       </c>
       <c r="F19" s="261"/>
-      <c r="G19" s="420"/>
+      <c r="G19" s="417"/>
       <c r="H19" s="262" t="s">
         <v>183</v>
       </c>
@@ -6836,15 +6841,15 @@
       <c r="B22" s="272"/>
       <c r="C22" s="273"/>
       <c r="D22" s="274"/>
-      <c r="E22" s="377"/>
-      <c r="F22" s="377"/>
-      <c r="G22" s="377"/>
-      <c r="H22" s="377"/>
-      <c r="I22" s="377"/>
-      <c r="J22" s="377"/>
-      <c r="K22" s="377"/>
-      <c r="L22" s="377"/>
-      <c r="M22" s="377"/>
+      <c r="E22" s="372"/>
+      <c r="F22" s="372"/>
+      <c r="G22" s="372"/>
+      <c r="H22" s="372"/>
+      <c r="I22" s="372"/>
+      <c r="J22" s="372"/>
+      <c r="K22" s="372"/>
+      <c r="L22" s="372"/>
+      <c r="M22" s="372"/>
       <c r="N22" s="216"/>
       <c r="P22" s="133"/>
       <c r="Q22" s="133"/>
@@ -7229,44 +7234,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A1" s="462"/>
-      <c r="B1" s="463"/>
-      <c r="C1" s="472" t="s">
+      <c r="A1" s="450"/>
+      <c r="B1" s="451"/>
+      <c r="C1" s="457" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="472"/>
-      <c r="E1" s="472"/>
-      <c r="F1" s="472"/>
-      <c r="G1" s="472"/>
-      <c r="H1" s="472"/>
-      <c r="I1" s="475" t="s">
+      <c r="D1" s="457"/>
+      <c r="E1" s="457"/>
+      <c r="F1" s="457"/>
+      <c r="G1" s="457"/>
+      <c r="H1" s="457"/>
+      <c r="I1" s="440" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="475"/>
+      <c r="J1" s="440"/>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="464"/>
-      <c r="B2" s="465"/>
-      <c r="C2" s="472"/>
-      <c r="D2" s="472"/>
-      <c r="E2" s="472"/>
-      <c r="F2" s="472"/>
-      <c r="G2" s="472"/>
-      <c r="H2" s="472"/>
-      <c r="I2" s="476" t="s">
+      <c r="A2" s="452"/>
+      <c r="B2" s="453"/>
+      <c r="C2" s="457"/>
+      <c r="D2" s="457"/>
+      <c r="E2" s="457"/>
+      <c r="F2" s="457"/>
+      <c r="G2" s="457"/>
+      <c r="H2" s="457"/>
+      <c r="I2" s="441" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="476"/>
+      <c r="J2" s="441"/>
     </row>
     <row r="3" spans="1:10" ht="33" customHeight="1">
-      <c r="A3" s="466"/>
-      <c r="B3" s="467"/>
-      <c r="C3" s="472"/>
-      <c r="D3" s="472"/>
-      <c r="E3" s="472"/>
-      <c r="F3" s="472"/>
-      <c r="G3" s="472"/>
-      <c r="H3" s="472"/>
+      <c r="A3" s="454"/>
+      <c r="B3" s="455"/>
+      <c r="C3" s="457"/>
+      <c r="D3" s="457"/>
+      <c r="E3" s="457"/>
+      <c r="F3" s="457"/>
+      <c r="G3" s="457"/>
+      <c r="H3" s="457"/>
       <c r="I3" s="65" t="s">
         <v>95</v>
       </c>
@@ -7357,13 +7362,13 @@
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="52"/>
-      <c r="B11" s="439" t="s">
+      <c r="B11" s="456" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="439" t="s">
+      <c r="C11" s="456" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="441" t="s">
+      <c r="D11" s="431" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="20" t="s">
@@ -7377,16 +7382,16 @@
     </row>
     <row r="12" spans="1:10" ht="75">
       <c r="A12" s="76"/>
-      <c r="B12" s="439"/>
-      <c r="C12" s="439"/>
-      <c r="D12" s="445"/>
+      <c r="B12" s="456"/>
+      <c r="C12" s="456"/>
+      <c r="D12" s="435"/>
       <c r="E12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="473" t="s">
+      <c r="F12" s="458" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="474"/>
+      <c r="G12" s="459"/>
       <c r="H12" s="15" t="s">
         <v>47</v>
       </c>
@@ -7397,18 +7402,18 @@
     </row>
     <row r="13" spans="1:10" ht="15.6">
       <c r="A13" s="76"/>
-      <c r="B13" s="439"/>
-      <c r="C13" s="439"/>
+      <c r="B13" s="456"/>
+      <c r="C13" s="456"/>
       <c r="D13" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="432" t="s">
+      <c r="F13" s="428" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="433"/>
+      <c r="G13" s="429"/>
       <c r="H13" s="5" t="s">
         <v>42</v>
       </c>
@@ -7431,10 +7436,10 @@
       <c r="E14" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="434" t="s">
+      <c r="F14" s="424" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="435"/>
+      <c r="G14" s="425"/>
       <c r="H14" s="81" t="s">
         <v>74</v>
       </c>
@@ -7449,8 +7454,8 @@
       <c r="C15" s="25"/>
       <c r="D15" s="59"/>
       <c r="E15" s="81"/>
-      <c r="F15" s="477"/>
-      <c r="G15" s="478"/>
+      <c r="F15" s="426"/>
+      <c r="G15" s="427"/>
       <c r="H15" s="81"/>
       <c r="I15" s="22"/>
       <c r="J15" s="72"/>
@@ -7493,10 +7498,10 @@
     </row>
     <row r="19" spans="1:10" s="28" customFormat="1" ht="20.25" customHeight="1">
       <c r="A19" s="52"/>
-      <c r="B19" s="468" t="s">
+      <c r="B19" s="436" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="468"/>
+      <c r="C19" s="436"/>
       <c r="D19" s="53" t="s">
         <v>76</v>
       </c>
@@ -7514,13 +7519,13 @@
     </row>
     <row r="21" spans="1:10" ht="18" customHeight="1">
       <c r="A21" s="52"/>
-      <c r="B21" s="439" t="s">
+      <c r="B21" s="456" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="439" t="s">
+      <c r="C21" s="456" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="469" t="s">
+      <c r="D21" s="437" t="s">
         <v>33</v>
       </c>
       <c r="E21" s="20" t="s">
@@ -7534,74 +7539,74 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="52"/>
-      <c r="B22" s="439"/>
-      <c r="C22" s="439"/>
-      <c r="D22" s="470"/>
-      <c r="E22" s="469" t="s">
+      <c r="B22" s="456"/>
+      <c r="C22" s="456"/>
+      <c r="D22" s="438"/>
+      <c r="E22" s="437" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="440" t="s">
+      <c r="F22" s="430" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="441"/>
-      <c r="H22" s="469" t="s">
+      <c r="G22" s="431"/>
+      <c r="H22" s="437" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="469" t="s">
+      <c r="I22" s="437" t="s">
         <v>46</v>
       </c>
       <c r="J22" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="52"/>
-      <c r="B23" s="439"/>
-      <c r="C23" s="439"/>
-      <c r="D23" s="470"/>
-      <c r="E23" s="470"/>
-      <c r="F23" s="442"/>
-      <c r="G23" s="443"/>
-      <c r="H23" s="470"/>
-      <c r="I23" s="470"/>
+      <c r="B23" s="456"/>
+      <c r="C23" s="456"/>
+      <c r="D23" s="438"/>
+      <c r="E23" s="438"/>
+      <c r="F23" s="432"/>
+      <c r="G23" s="433"/>
+      <c r="H23" s="438"/>
+      <c r="I23" s="438"/>
       <c r="J23" s="72"/>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="A24" s="52"/>
-      <c r="B24" s="439"/>
-      <c r="C24" s="439"/>
-      <c r="D24" s="470"/>
-      <c r="E24" s="470"/>
-      <c r="F24" s="442"/>
-      <c r="G24" s="443"/>
-      <c r="H24" s="470"/>
-      <c r="I24" s="470"/>
+      <c r="B24" s="456"/>
+      <c r="C24" s="456"/>
+      <c r="D24" s="438"/>
+      <c r="E24" s="438"/>
+      <c r="F24" s="432"/>
+      <c r="G24" s="433"/>
+      <c r="H24" s="438"/>
+      <c r="I24" s="438"/>
       <c r="J24" s="72"/>
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="52"/>
-      <c r="B25" s="439"/>
-      <c r="C25" s="439"/>
-      <c r="D25" s="471"/>
-      <c r="E25" s="471"/>
-      <c r="F25" s="444"/>
-      <c r="G25" s="445"/>
-      <c r="H25" s="471"/>
-      <c r="I25" s="471"/>
+      <c r="B25" s="456"/>
+      <c r="C25" s="456"/>
+      <c r="D25" s="439"/>
+      <c r="E25" s="439"/>
+      <c r="F25" s="434"/>
+      <c r="G25" s="435"/>
+      <c r="H25" s="439"/>
+      <c r="I25" s="439"/>
       <c r="J25" s="72"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="52"/>
-      <c r="B26" s="439"/>
-      <c r="C26" s="439"/>
+      <c r="B26" s="456"/>
+      <c r="C26" s="456"/>
       <c r="D26" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="432" t="s">
+      <c r="F26" s="428" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="433"/>
+      <c r="G26" s="429"/>
       <c r="H26" s="5" t="s">
         <v>42</v>
       </c>
@@ -7624,10 +7629,10 @@
       <c r="E27" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="434" t="s">
+      <c r="F27" s="424" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="435"/>
+      <c r="G27" s="425"/>
       <c r="H27" s="81" t="s">
         <v>74</v>
       </c>
@@ -7642,8 +7647,8 @@
       <c r="C28" s="17"/>
       <c r="D28" s="60"/>
       <c r="E28" s="81"/>
-      <c r="F28" s="477"/>
-      <c r="G28" s="478"/>
+      <c r="F28" s="426"/>
+      <c r="G28" s="427"/>
       <c r="H28" s="81"/>
       <c r="I28" s="82"/>
       <c r="J28" s="72"/>
@@ -7764,13 +7769,13 @@
     </row>
     <row r="38" spans="1:10" ht="18" customHeight="1">
       <c r="A38" s="52"/>
-      <c r="B38" s="439" t="s">
+      <c r="B38" s="456" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="439" t="s">
+      <c r="C38" s="456" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="441" t="s">
+      <c r="D38" s="431" t="s">
         <v>33</v>
       </c>
       <c r="E38" s="20" t="s">
@@ -7784,74 +7789,74 @@
     </row>
     <row r="39" spans="1:10" ht="18" customHeight="1">
       <c r="A39" s="52"/>
-      <c r="B39" s="439"/>
-      <c r="C39" s="439"/>
-      <c r="D39" s="443"/>
-      <c r="E39" s="468" t="s">
+      <c r="B39" s="456"/>
+      <c r="C39" s="456"/>
+      <c r="D39" s="433"/>
+      <c r="E39" s="436" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="440" t="s">
+      <c r="F39" s="430" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="441"/>
-      <c r="H39" s="468" t="s">
+      <c r="G39" s="431"/>
+      <c r="H39" s="436" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="468" t="s">
+      <c r="I39" s="436" t="s">
         <v>29</v>
       </c>
       <c r="J39" s="72"/>
     </row>
     <row r="40" spans="1:10" ht="18" customHeight="1">
       <c r="A40" s="52"/>
-      <c r="B40" s="439"/>
-      <c r="C40" s="439"/>
-      <c r="D40" s="443"/>
-      <c r="E40" s="468"/>
-      <c r="F40" s="442"/>
-      <c r="G40" s="443"/>
-      <c r="H40" s="468"/>
-      <c r="I40" s="468"/>
+      <c r="B40" s="456"/>
+      <c r="C40" s="456"/>
+      <c r="D40" s="433"/>
+      <c r="E40" s="436"/>
+      <c r="F40" s="432"/>
+      <c r="G40" s="433"/>
+      <c r="H40" s="436"/>
+      <c r="I40" s="436"/>
       <c r="J40" s="72"/>
     </row>
     <row r="41" spans="1:10" ht="18" customHeight="1">
       <c r="A41" s="52"/>
-      <c r="B41" s="439"/>
-      <c r="C41" s="439"/>
-      <c r="D41" s="443"/>
-      <c r="E41" s="468"/>
-      <c r="F41" s="442"/>
-      <c r="G41" s="443"/>
-      <c r="H41" s="468"/>
-      <c r="I41" s="468"/>
+      <c r="B41" s="456"/>
+      <c r="C41" s="456"/>
+      <c r="D41" s="433"/>
+      <c r="E41" s="436"/>
+      <c r="F41" s="432"/>
+      <c r="G41" s="433"/>
+      <c r="H41" s="436"/>
+      <c r="I41" s="436"/>
       <c r="J41" s="72"/>
     </row>
     <row r="42" spans="1:10" ht="15">
       <c r="A42" s="52"/>
-      <c r="B42" s="439"/>
-      <c r="C42" s="439"/>
-      <c r="D42" s="445"/>
-      <c r="E42" s="468"/>
-      <c r="F42" s="444"/>
-      <c r="G42" s="445"/>
-      <c r="H42" s="468"/>
-      <c r="I42" s="468"/>
+      <c r="B42" s="456"/>
+      <c r="C42" s="456"/>
+      <c r="D42" s="435"/>
+      <c r="E42" s="436"/>
+      <c r="F42" s="434"/>
+      <c r="G42" s="435"/>
+      <c r="H42" s="436"/>
+      <c r="I42" s="436"/>
       <c r="J42" s="72"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1">
       <c r="A43" s="52"/>
-      <c r="B43" s="439"/>
-      <c r="C43" s="439"/>
+      <c r="B43" s="456"/>
+      <c r="C43" s="456"/>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="432" t="s">
+      <c r="F43" s="428" t="s">
         <v>26</v>
       </c>
-      <c r="G43" s="433"/>
+      <c r="G43" s="429"/>
       <c r="H43" s="5" t="s">
         <v>25</v>
       </c>
@@ -7874,10 +7879,10 @@
       <c r="E44" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="F44" s="453" t="s">
+      <c r="F44" s="471" t="s">
         <v>59</v>
       </c>
-      <c r="G44" s="454"/>
+      <c r="G44" s="472"/>
       <c r="H44" s="84" t="s">
         <v>74</v>
       </c>
@@ -7892,8 +7897,8 @@
       <c r="C45" s="17"/>
       <c r="D45" s="47"/>
       <c r="E45" s="85"/>
-      <c r="F45" s="455"/>
-      <c r="G45" s="456"/>
+      <c r="F45" s="473"/>
+      <c r="G45" s="474"/>
       <c r="H45" s="63"/>
       <c r="I45" s="63"/>
       <c r="J45" s="72"/>
@@ -7901,12 +7906,12 @@
     <row r="46" spans="1:10" ht="15">
       <c r="A46" s="52"/>
       <c r="B46" s="8"/>
-      <c r="C46" s="452"/>
-      <c r="D46" s="452"/>
-      <c r="E46" s="452"/>
-      <c r="F46" s="452"/>
-      <c r="G46" s="452"/>
-      <c r="H46" s="452"/>
+      <c r="C46" s="470"/>
+      <c r="D46" s="470"/>
+      <c r="E46" s="470"/>
+      <c r="F46" s="470"/>
+      <c r="G46" s="470"/>
+      <c r="H46" s="470"/>
       <c r="I46" s="12"/>
       <c r="J46" s="72"/>
     </row>
@@ -7914,11 +7919,11 @@
       <c r="A47" s="52"/>
       <c r="C47" s="38"/>
       <c r="D47" s="42"/>
-      <c r="E47" s="457" t="s">
+      <c r="E47" s="442" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="457"/>
-      <c r="G47" s="457"/>
+      <c r="F47" s="442"/>
+      <c r="G47" s="442"/>
       <c r="H47" s="62" t="s">
         <v>77</v>
       </c>
@@ -7929,11 +7934,11 @@
     </row>
     <row r="48" spans="1:10" ht="18" customHeight="1">
       <c r="A48" s="52"/>
-      <c r="E48" s="457" t="s">
+      <c r="E48" s="442" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="457"/>
-      <c r="G48" s="457"/>
+      <c r="F48" s="442"/>
+      <c r="G48" s="442"/>
       <c r="H48" s="61" t="s">
         <v>78</v>
       </c>
@@ -7950,11 +7955,11 @@
     </row>
     <row r="50" spans="1:10" ht="15">
       <c r="A50" s="52"/>
-      <c r="E50" s="427" t="s">
+      <c r="E50" s="475" t="s">
         <v>20</v>
       </c>
-      <c r="F50" s="427"/>
-      <c r="G50" s="427"/>
+      <c r="F50" s="475"/>
+      <c r="G50" s="475"/>
       <c r="H50" s="54" t="s">
         <v>79</v>
       </c>
@@ -7990,87 +7995,87 @@
     </row>
     <row r="54" spans="1:10" ht="15">
       <c r="A54" s="52"/>
-      <c r="B54" s="449" t="s">
+      <c r="B54" s="467" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="449" t="s">
+      <c r="C54" s="467" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="446" t="s">
+      <c r="D54" s="464" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="447"/>
-      <c r="F54" s="447"/>
-      <c r="G54" s="447"/>
-      <c r="H54" s="448"/>
+      <c r="E54" s="465"/>
+      <c r="F54" s="465"/>
+      <c r="G54" s="465"/>
+      <c r="H54" s="466"/>
       <c r="J54" s="72"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1">
       <c r="A55" s="52"/>
-      <c r="B55" s="450"/>
-      <c r="C55" s="450"/>
-      <c r="D55" s="428" t="s">
+      <c r="B55" s="468"/>
+      <c r="C55" s="468"/>
+      <c r="D55" s="443" t="s">
         <v>15</v>
       </c>
-      <c r="E55" s="428" t="s">
+      <c r="E55" s="443" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="458" t="s">
+      <c r="F55" s="446" t="s">
         <v>13</v>
       </c>
-      <c r="G55" s="459"/>
-      <c r="H55" s="428" t="s">
+      <c r="G55" s="447"/>
+      <c r="H55" s="443" t="s">
         <v>12</v>
       </c>
       <c r="J55" s="72"/>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1">
       <c r="A56" s="52"/>
-      <c r="B56" s="450"/>
-      <c r="C56" s="450"/>
-      <c r="D56" s="429"/>
-      <c r="E56" s="429"/>
-      <c r="F56" s="460"/>
-      <c r="G56" s="461"/>
-      <c r="H56" s="429"/>
+      <c r="B56" s="468"/>
+      <c r="C56" s="468"/>
+      <c r="D56" s="444"/>
+      <c r="E56" s="444"/>
+      <c r="F56" s="448"/>
+      <c r="G56" s="449"/>
+      <c r="H56" s="444"/>
       <c r="J56" s="72"/>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1">
       <c r="A57" s="52"/>
-      <c r="B57" s="450"/>
-      <c r="C57" s="450"/>
-      <c r="D57" s="429"/>
-      <c r="E57" s="429"/>
-      <c r="F57" s="460"/>
-      <c r="G57" s="461"/>
-      <c r="H57" s="429"/>
+      <c r="B57" s="468"/>
+      <c r="C57" s="468"/>
+      <c r="D57" s="444"/>
+      <c r="E57" s="444"/>
+      <c r="F57" s="448"/>
+      <c r="G57" s="449"/>
+      <c r="H57" s="444"/>
       <c r="J57" s="72"/>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1">
       <c r="A58" s="52"/>
-      <c r="B58" s="450"/>
-      <c r="C58" s="450"/>
-      <c r="D58" s="430"/>
-      <c r="E58" s="430"/>
-      <c r="F58" s="460"/>
-      <c r="G58" s="461"/>
-      <c r="H58" s="430"/>
+      <c r="B58" s="468"/>
+      <c r="C58" s="468"/>
+      <c r="D58" s="445"/>
+      <c r="E58" s="445"/>
+      <c r="F58" s="448"/>
+      <c r="G58" s="449"/>
+      <c r="H58" s="445"/>
       <c r="J58" s="72"/>
     </row>
     <row r="59" spans="1:10" ht="15.75" customHeight="1">
       <c r="A59" s="52"/>
-      <c r="B59" s="451"/>
-      <c r="C59" s="451"/>
+      <c r="B59" s="469"/>
+      <c r="C59" s="469"/>
       <c r="D59" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F59" s="432" t="s">
+      <c r="F59" s="428" t="s">
         <v>9</v>
       </c>
-      <c r="G59" s="433"/>
+      <c r="G59" s="429"/>
       <c r="H59" s="5" t="s">
         <v>8</v>
       </c>
@@ -8090,10 +8095,10 @@
       <c r="E60" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="F60" s="434" t="s">
+      <c r="F60" s="424" t="s">
         <v>90</v>
       </c>
-      <c r="G60" s="435"/>
+      <c r="G60" s="425"/>
       <c r="H60" s="55" t="s">
         <v>91</v>
       </c>
@@ -8200,13 +8205,13 @@
     <row r="68" spans="1:10" ht="15" customHeight="1">
       <c r="A68" s="52"/>
       <c r="B68" s="8"/>
-      <c r="C68" s="436" t="s">
+      <c r="C68" s="460" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="437" t="s">
+      <c r="D68" s="461" t="s">
         <v>86</v>
       </c>
-      <c r="E68" s="438" t="s">
+      <c r="E68" s="462" t="s">
         <v>0</v>
       </c>
       <c r="F68" s="4"/>
@@ -8218,9 +8223,9 @@
     <row r="69" spans="1:10" ht="15" customHeight="1">
       <c r="A69" s="52"/>
       <c r="B69" s="8"/>
-      <c r="C69" s="436"/>
-      <c r="D69" s="437"/>
-      <c r="E69" s="438"/>
+      <c r="C69" s="460"/>
+      <c r="D69" s="461"/>
+      <c r="E69" s="462"/>
       <c r="F69" s="4"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
@@ -8324,15 +8329,15 @@
         <v>93</v>
       </c>
       <c r="D77" s="88"/>
-      <c r="E77" s="431" t="s">
+      <c r="E77" s="463" t="s">
         <v>99</v>
       </c>
-      <c r="F77" s="431"/>
+      <c r="F77" s="463"/>
       <c r="G77" s="89"/>
-      <c r="H77" s="431" t="s">
+      <c r="H77" s="463" t="s">
         <v>97</v>
       </c>
-      <c r="I77" s="431"/>
+      <c r="I77" s="463"/>
       <c r="J77" s="72"/>
     </row>
     <row r="78" spans="1:10" ht="18" customHeight="1">
@@ -8396,19 +8401,27 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F22:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="F39:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="D54:H54"/>
+    <mergeCell ref="C54:C59"/>
+    <mergeCell ref="B54:B59"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="E47:G47"/>
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="D55:D58"/>
     <mergeCell ref="E55:E58"/>
@@ -8425,27 +8438,19 @@
     <mergeCell ref="C1:H3"/>
     <mergeCell ref="E39:E42"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="F39:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="D54:H54"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="B54:B59"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="C38:C43"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F22:G25"/>
+    <mergeCell ref="F26:G26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8463,7 +8468,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.88671875" defaultRowHeight="14.4"/>
@@ -8478,34 +8483,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A1" s="489"/>
-      <c r="B1" s="490"/>
-      <c r="C1" s="491" t="s">
+      <c r="A1" s="476"/>
+      <c r="B1" s="477"/>
+      <c r="C1" s="478" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="492"/>
-      <c r="E1" s="493" t="s">
+      <c r="D1" s="479"/>
+      <c r="E1" s="480" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="494"/>
+      <c r="F1" s="481"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="495"/>
-      <c r="B2" s="496"/>
-      <c r="C2" s="497" t="s">
+      <c r="A2" s="482"/>
+      <c r="B2" s="483"/>
+      <c r="C2" s="484" t="s">
         <v>202</v>
       </c>
-      <c r="D2" s="498"/>
-      <c r="E2" s="499" t="s">
+      <c r="D2" s="485"/>
+      <c r="E2" s="486" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="500"/>
+      <c r="F2" s="487"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="480" t="s">
+      <c r="A3" s="489" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="481"/>
+      <c r="B3" s="490"/>
       <c r="C3" s="316"/>
       <c r="D3" s="317"/>
       <c r="E3" s="318"/>
@@ -8519,12 +8524,12 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="322"/>
-      <c r="B5" s="482" t="s">
+      <c r="B5" s="491" t="s">
         <v>205</v>
       </c>
-      <c r="C5" s="482"/>
-      <c r="D5" s="482"/>
-      <c r="E5" s="482"/>
+      <c r="C5" s="491"/>
+      <c r="D5" s="491"/>
+      <c r="E5" s="491"/>
       <c r="F5" s="321"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
@@ -8535,7 +8540,7 @@
     </row>
     <row r="7" spans="1:6" ht="40.200000000000003">
       <c r="A7" s="322"/>
-      <c r="B7" s="483" t="s">
+      <c r="B7" s="492" t="s">
         <v>206</v>
       </c>
       <c r="C7" s="323" t="s">
@@ -8544,107 +8549,107 @@
       <c r="D7" s="324" t="s">
         <v>208</v>
       </c>
-      <c r="E7" s="325" t="s">
+      <c r="E7" s="505" t="s">
         <v>209</v>
       </c>
-      <c r="F7" s="321"/>
+      <c r="F7" s="505"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="322"/>
-      <c r="B8" s="484"/>
-      <c r="C8" s="326" t="s">
+      <c r="B8" s="493"/>
+      <c r="C8" s="325" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="327" t="s">
+      <c r="D8" s="326" t="s">
         <v>211</v>
       </c>
-      <c r="E8" s="328" t="s">
+      <c r="E8" s="506" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="321"/>
+      <c r="F8" s="506"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="322"/>
-      <c r="B9" s="484"/>
-      <c r="C9" s="326" t="s">
+      <c r="B9" s="493"/>
+      <c r="C9" s="325" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="486" t="s">
+      <c r="D9" s="495" t="s">
         <v>214</v>
       </c>
-      <c r="E9" s="486" t="s">
+      <c r="E9" s="508" t="s">
         <v>214</v>
       </c>
-      <c r="F9" s="321"/>
+      <c r="F9" s="508"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="322"/>
-      <c r="B10" s="485"/>
-      <c r="C10" s="328" t="s">
+      <c r="B10" s="494"/>
+      <c r="C10" s="327" t="s">
         <v>215</v>
       </c>
-      <c r="D10" s="487"/>
-      <c r="E10" s="487"/>
-      <c r="F10" s="321"/>
-    </row>
-    <row r="11" spans="1:6" s="334" customFormat="1" ht="10.199999999999999">
-      <c r="A11" s="329"/>
-      <c r="B11" s="330" t="s">
+      <c r="D10" s="496"/>
+      <c r="E10" s="508"/>
+      <c r="F10" s="508"/>
+    </row>
+    <row r="11" spans="1:6" s="332" customFormat="1" ht="10.199999999999999">
+      <c r="A11" s="328"/>
+      <c r="B11" s="329" t="s">
         <v>249</v>
       </c>
-      <c r="C11" s="330" t="s">
+      <c r="C11" s="329" t="s">
         <v>291</v>
       </c>
-      <c r="D11" s="332" t="s">
+      <c r="D11" s="331" t="s">
         <v>293</v>
       </c>
-      <c r="E11" s="331" t="s">
+      <c r="E11" s="509" t="s">
         <v>295</v>
       </c>
-      <c r="F11" s="333"/>
-    </row>
-    <row r="12" spans="1:6" s="334" customFormat="1" ht="10.199999999999999">
-      <c r="A12" s="329"/>
-      <c r="B12" s="335"/>
-      <c r="C12" s="331"/>
-      <c r="D12" s="332"/>
-      <c r="E12" s="331"/>
-      <c r="F12" s="333"/>
+      <c r="F11" s="509"/>
+    </row>
+    <row r="12" spans="1:6" s="332" customFormat="1" ht="10.199999999999999">
+      <c r="A12" s="328"/>
+      <c r="B12" s="333"/>
+      <c r="C12" s="330"/>
+      <c r="D12" s="331"/>
+      <c r="E12" s="509"/>
+      <c r="F12" s="509"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="322"/>
-      <c r="B13" s="336"/>
-      <c r="C13" s="337"/>
-      <c r="D13" s="338">
+      <c r="B13" s="334"/>
+      <c r="C13" s="335"/>
+      <c r="D13" s="336">
         <f>SUM(D11:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="331">
+      <c r="E13" s="509">
         <f>SUM(E11:E12)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="321"/>
+      <c r="F13" s="509"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="322"/>
       <c r="B14" s="315"/>
-      <c r="C14" s="339"/>
-      <c r="D14" s="340"/>
-      <c r="E14" s="341"/>
+      <c r="C14" s="337"/>
+      <c r="D14" s="338"/>
+      <c r="E14" s="510"/>
       <c r="F14" s="321"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="322"/>
-      <c r="B15" s="342"/>
-      <c r="C15" s="343" t="s">
+      <c r="B15" s="339"/>
+      <c r="C15" s="340" t="s">
         <v>216</v>
       </c>
-      <c r="D15" s="337"/>
-      <c r="E15" s="344">
+      <c r="D15" s="335"/>
+      <c r="E15" s="341">
         <f>SUM(E11:E12)*42/1000000</f>
         <v>0</v>
       </c>
-      <c r="F15" s="345" t="s">
+      <c r="F15" s="342" t="s">
         <v>217</v>
       </c>
     </row>
@@ -8657,7 +8662,7 @@
       <c r="F17" s="321"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="346" t="s">
+      <c r="A18" s="343" t="s">
         <v>218</v>
       </c>
       <c r="F18" s="321"/>
@@ -8667,13 +8672,13 @@
       <c r="F19" s="321"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="347" t="s">
+      <c r="A20" s="344" t="s">
         <v>219</v>
       </c>
       <c r="F20" s="321"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="347" t="s">
+      <c r="A21" s="344" t="s">
         <v>220</v>
       </c>
       <c r="F21" s="321"/>
@@ -8683,19 +8688,19 @@
       <c r="F22" s="321"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="348" t="s">
+      <c r="A23" s="345" t="s">
         <v>221</v>
       </c>
       <c r="F23" s="321"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="347" t="s">
+      <c r="A24" s="344" t="s">
         <v>222</v>
       </c>
       <c r="F24" s="321"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="347" t="s">
+      <c r="A25" s="344" t="s">
         <v>223</v>
       </c>
       <c r="F25" s="321"/>
@@ -8708,14 +8713,14 @@
       <c r="A27" s="322" t="s">
         <v>224</v>
       </c>
-      <c r="D27" s="349"/>
+      <c r="D27" s="346"/>
       <c r="F27" s="321"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="347" t="s">
+      <c r="A28" s="344" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="349"/>
+      <c r="D28" s="346"/>
       <c r="F28" s="321"/>
     </row>
     <row r="29" spans="1:6">
@@ -8723,59 +8728,64 @@
       <c r="F29" s="321"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="350" t="s">
+      <c r="A30" s="347" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="351" t="s">
+      <c r="B30" s="348" t="s">
         <v>226</v>
       </c>
-      <c r="C30" s="352" t="s">
+      <c r="C30" s="349" t="s">
         <v>227</v>
       </c>
-      <c r="D30" s="351" t="s">
+      <c r="D30" s="348" t="s">
         <v>228</v>
       </c>
-      <c r="E30" s="488" t="s">
+      <c r="E30" s="497" t="s">
         <v>229</v>
       </c>
-      <c r="F30" s="488"/>
+      <c r="F30" s="497"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="353">
+      <c r="A31" s="350">
         <v>0</v>
       </c>
-      <c r="B31" s="354">
+      <c r="B31" s="351">
         <v>41331</v>
       </c>
-      <c r="C31" s="352" t="s">
+      <c r="C31" s="349" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="351" t="s">
+      <c r="D31" s="348" t="s">
         <v>231</v>
       </c>
-      <c r="E31" s="479" t="s">
+      <c r="E31" s="488" t="s">
         <v>232</v>
       </c>
-      <c r="F31" s="479"/>
+      <c r="F31" s="488"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="349"/>
+      <c r="A32" s="346"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8788,7 +8798,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.88671875" defaultRowHeight="14.4"/>
@@ -8796,41 +8806,41 @@
     <col min="1" max="1" width="9.109375" style="315" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" style="320" customWidth="1"/>
     <col min="3" max="3" width="22" style="315" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="315" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="315" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="315" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" style="315" customWidth="1"/>
     <col min="7" max="16384" width="14.88671875" style="315"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24.75" customHeight="1">
-      <c r="A1" s="489"/>
-      <c r="B1" s="490"/>
-      <c r="C1" s="491" t="s">
+      <c r="A1" s="476"/>
+      <c r="B1" s="477"/>
+      <c r="C1" s="478" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="492"/>
-      <c r="E1" s="493" t="s">
+      <c r="D1" s="479"/>
+      <c r="E1" s="480" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="494"/>
+      <c r="F1" s="481"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="495"/>
-      <c r="B2" s="496"/>
-      <c r="C2" s="497" t="s">
+      <c r="A2" s="482"/>
+      <c r="B2" s="483"/>
+      <c r="C2" s="484" t="s">
         <v>202</v>
       </c>
-      <c r="D2" s="498"/>
-      <c r="E2" s="499" t="s">
+      <c r="D2" s="485"/>
+      <c r="E2" s="486" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="500"/>
+      <c r="F2" s="487"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="480" t="s">
+      <c r="A3" s="489" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="481"/>
+      <c r="B3" s="490"/>
       <c r="C3" s="316"/>
       <c r="D3" s="317"/>
       <c r="E3" s="318"/>
@@ -8844,12 +8854,12 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="322"/>
-      <c r="B5" s="482" t="s">
+      <c r="B5" s="491" t="s">
         <v>233</v>
       </c>
-      <c r="C5" s="482"/>
-      <c r="D5" s="482"/>
-      <c r="E5" s="482"/>
+      <c r="C5" s="491"/>
+      <c r="D5" s="491"/>
+      <c r="E5" s="491"/>
       <c r="F5" s="321"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
@@ -8860,7 +8870,7 @@
     </row>
     <row r="7" spans="1:6" ht="40.200000000000003">
       <c r="A7" s="322"/>
-      <c r="B7" s="483" t="s">
+      <c r="B7" s="492" t="s">
         <v>206</v>
       </c>
       <c r="C7" s="323" t="s">
@@ -8869,107 +8879,107 @@
       <c r="D7" s="324" t="s">
         <v>208</v>
       </c>
-      <c r="E7" s="325" t="s">
+      <c r="E7" s="505" t="s">
         <v>209</v>
       </c>
-      <c r="F7" s="321"/>
+      <c r="F7" s="505"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="322"/>
-      <c r="B8" s="484"/>
-      <c r="C8" s="326" t="s">
+      <c r="B8" s="493"/>
+      <c r="C8" s="325" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="327" t="s">
+      <c r="D8" s="326" t="s">
         <v>211</v>
       </c>
-      <c r="E8" s="328" t="s">
+      <c r="E8" s="506" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="321"/>
+      <c r="F8" s="506"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="322"/>
-      <c r="B9" s="484"/>
-      <c r="C9" s="326" t="s">
+      <c r="B9" s="493"/>
+      <c r="C9" s="325" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="486" t="s">
+      <c r="D9" s="495" t="s">
         <v>181</v>
       </c>
-      <c r="E9" s="486" t="s">
+      <c r="E9" s="508" t="s">
         <v>181</v>
       </c>
-      <c r="F9" s="321"/>
+      <c r="F9" s="508"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="322"/>
-      <c r="B10" s="485"/>
-      <c r="C10" s="328" t="s">
+      <c r="B10" s="494"/>
+      <c r="C10" s="327" t="s">
         <v>215</v>
       </c>
-      <c r="D10" s="487"/>
-      <c r="E10" s="487"/>
-      <c r="F10" s="321"/>
-    </row>
-    <row r="11" spans="1:6" s="334" customFormat="1" ht="10.199999999999999">
-      <c r="A11" s="329"/>
-      <c r="B11" s="330" t="s">
+      <c r="D10" s="496"/>
+      <c r="E10" s="508"/>
+      <c r="F10" s="508"/>
+    </row>
+    <row r="11" spans="1:6" s="332" customFormat="1" ht="10.199999999999999">
+      <c r="A11" s="328"/>
+      <c r="B11" s="329" t="s">
         <v>249</v>
       </c>
-      <c r="C11" s="330" t="s">
+      <c r="C11" s="329" t="s">
         <v>291</v>
       </c>
-      <c r="D11" s="355" t="s">
+      <c r="D11" s="352" t="s">
         <v>294</v>
       </c>
-      <c r="E11" s="331" t="s">
+      <c r="E11" s="509" t="s">
         <v>296</v>
       </c>
-      <c r="F11" s="333"/>
-    </row>
-    <row r="12" spans="1:6" s="334" customFormat="1" ht="10.199999999999999">
-      <c r="A12" s="329"/>
-      <c r="B12" s="335"/>
-      <c r="C12" s="331"/>
-      <c r="D12" s="332"/>
-      <c r="E12" s="331"/>
-      <c r="F12" s="333"/>
+      <c r="F11" s="509"/>
+    </row>
+    <row r="12" spans="1:6" s="332" customFormat="1" ht="10.199999999999999">
+      <c r="A12" s="328"/>
+      <c r="B12" s="333"/>
+      <c r="C12" s="330"/>
+      <c r="D12" s="331"/>
+      <c r="E12" s="509"/>
+      <c r="F12" s="509"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="322"/>
-      <c r="B13" s="336"/>
-      <c r="C13" s="337"/>
-      <c r="D13" s="338">
+      <c r="B13" s="334"/>
+      <c r="C13" s="335"/>
+      <c r="D13" s="336">
         <f>SUM(D11:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="331">
+      <c r="E13" s="509">
         <f>SUM(E11:E12)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="321"/>
+      <c r="F13" s="509"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="322"/>
       <c r="B14" s="315"/>
-      <c r="C14" s="339"/>
-      <c r="D14" s="340"/>
-      <c r="E14" s="341"/>
+      <c r="C14" s="337"/>
+      <c r="D14" s="338"/>
+      <c r="E14" s="510"/>
       <c r="F14" s="321"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="322"/>
-      <c r="B15" s="342"/>
-      <c r="C15" s="343" t="s">
+      <c r="B15" s="339"/>
+      <c r="C15" s="340" t="s">
         <v>216</v>
       </c>
-      <c r="D15" s="337"/>
-      <c r="E15" s="344">
+      <c r="D15" s="335"/>
+      <c r="E15" s="341">
         <f>SUM(E11:E12)*42/1000000</f>
         <v>0</v>
       </c>
-      <c r="F15" s="345" t="s">
+      <c r="F15" s="342" t="s">
         <v>217</v>
       </c>
     </row>
@@ -8982,7 +8992,7 @@
       <c r="F17" s="321"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="346" t="s">
+      <c r="A18" s="343" t="s">
         <v>234</v>
       </c>
       <c r="F18" s="321"/>
@@ -8992,13 +9002,13 @@
       <c r="F19" s="321"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="347" t="s">
+      <c r="A20" s="344" t="s">
         <v>235</v>
       </c>
       <c r="F20" s="321"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="347" t="s">
+      <c r="A21" s="344" t="s">
         <v>220</v>
       </c>
       <c r="F21" s="321"/>
@@ -9008,19 +9018,19 @@
       <c r="F22" s="321"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="348" t="s">
+      <c r="A23" s="345" t="s">
         <v>221</v>
       </c>
       <c r="F23" s="321"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="347" t="s">
+      <c r="A24" s="344" t="s">
         <v>222</v>
       </c>
       <c r="F24" s="321"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="347" t="s">
+      <c r="A25" s="344" t="s">
         <v>223</v>
       </c>
       <c r="F25" s="321"/>
@@ -9033,14 +9043,14 @@
       <c r="A27" s="322" t="s">
         <v>224</v>
       </c>
-      <c r="D27" s="349"/>
+      <c r="D27" s="346"/>
       <c r="F27" s="321"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="347" t="s">
+      <c r="A28" s="344" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="349"/>
+      <c r="D28" s="346"/>
       <c r="F28" s="321"/>
     </row>
     <row r="29" spans="1:6">
@@ -9048,59 +9058,64 @@
       <c r="F29" s="321"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="350" t="s">
+      <c r="A30" s="347" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="351" t="s">
+      <c r="B30" s="348" t="s">
         <v>226</v>
       </c>
-      <c r="C30" s="352" t="s">
+      <c r="C30" s="349" t="s">
         <v>227</v>
       </c>
-      <c r="D30" s="351" t="s">
+      <c r="D30" s="348" t="s">
         <v>228</v>
       </c>
-      <c r="E30" s="488" t="s">
+      <c r="E30" s="497" t="s">
         <v>229</v>
       </c>
-      <c r="F30" s="488"/>
+      <c r="F30" s="497"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="353">
+      <c r="A31" s="350">
         <v>0</v>
       </c>
-      <c r="B31" s="354">
+      <c r="B31" s="351">
         <v>41331</v>
       </c>
-      <c r="C31" s="352" t="s">
+      <c r="C31" s="349" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="351" t="s">
+      <c r="D31" s="348" t="s">
         <v>231</v>
       </c>
-      <c r="E31" s="479" t="s">
+      <c r="E31" s="488" t="s">
         <v>232</v>
       </c>
-      <c r="F31" s="479"/>
+      <c r="F31" s="488"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="349"/>
+      <c r="A32" s="346"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E9:F10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9113,7 +9128,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.88671875" defaultRowHeight="14.4"/>
@@ -9121,7 +9136,7 @@
     <col min="1" max="1" width="14.88671875" style="315"/>
     <col min="2" max="2" width="15.109375" style="315" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="320" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="315" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="315" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="315" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="315" customWidth="1"/>
     <col min="7" max="16384" width="14.88671875" style="315"/>
@@ -9129,35 +9144,35 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="319"/>
-      <c r="B1" s="356"/>
-      <c r="C1" s="491" t="s">
+      <c r="B1" s="353"/>
+      <c r="C1" s="478" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="505"/>
-      <c r="E1" s="493" t="s">
+      <c r="D1" s="498"/>
+      <c r="E1" s="480" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="494"/>
+      <c r="F1" s="481"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="322"/>
-      <c r="B2" s="357"/>
-      <c r="C2" s="497" t="s">
+      <c r="B2" s="354"/>
+      <c r="C2" s="484" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="506"/>
-      <c r="E2" s="499" t="s">
+      <c r="D2" s="499"/>
+      <c r="E2" s="486" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="500"/>
+      <c r="F2" s="487"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="480" t="s">
+      <c r="A3" s="489" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="481"/>
+      <c r="B3" s="490"/>
       <c r="C3" s="316"/>
-      <c r="D3" s="358"/>
+      <c r="D3" s="355"/>
       <c r="E3" s="318"/>
       <c r="F3" s="317"/>
     </row>
@@ -9167,12 +9182,12 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="322"/>
-      <c r="B5" s="359" t="s">
+      <c r="B5" s="356" t="s">
         <v>237</v>
       </c>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
+      <c r="C5" s="357"/>
+      <c r="D5" s="357"/>
+      <c r="E5" s="357"/>
       <c r="F5" s="321"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1">
@@ -9181,105 +9196,105 @@
     </row>
     <row r="7" spans="1:6" ht="26.4">
       <c r="A7" s="322"/>
-      <c r="B7" s="361"/>
-      <c r="C7" s="362" t="s">
+      <c r="B7" s="358"/>
+      <c r="C7" s="359" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="363" t="s">
+      <c r="D7" s="360" t="s">
         <v>238</v>
       </c>
-      <c r="E7" s="364" t="s">
+      <c r="E7" s="505" t="s">
         <v>209</v>
       </c>
-      <c r="F7" s="321"/>
+      <c r="F7" s="505"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="322"/>
-      <c r="B8" s="365"/>
-      <c r="C8" s="326" t="s">
+      <c r="B8" s="361"/>
+      <c r="C8" s="325" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="366" t="s">
+      <c r="D8" s="362" t="s">
         <v>211</v>
       </c>
-      <c r="E8" s="367" t="s">
+      <c r="E8" s="506" t="s">
         <v>239</v>
       </c>
-      <c r="F8" s="321"/>
+      <c r="F8" s="506"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="322"/>
-      <c r="B9" s="368" t="s">
+      <c r="B9" s="363" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="326" t="s">
+      <c r="C9" s="325" t="s">
         <v>240</v>
       </c>
-      <c r="D9" s="486" t="s">
+      <c r="D9" s="495" t="s">
         <v>144</v>
       </c>
-      <c r="E9" s="486" t="s">
+      <c r="E9" s="508" t="s">
         <v>144</v>
       </c>
-      <c r="F9" s="321"/>
+      <c r="F9" s="508"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="322"/>
-      <c r="B10" s="365"/>
-      <c r="C10" s="326" t="s">
+      <c r="B10" s="361"/>
+      <c r="C10" s="325" t="s">
         <v>241</v>
       </c>
-      <c r="D10" s="507"/>
-      <c r="E10" s="507"/>
-      <c r="F10" s="321"/>
+      <c r="D10" s="500"/>
+      <c r="E10" s="508"/>
+      <c r="F10" s="508"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="322"/>
-      <c r="B11" s="369"/>
-      <c r="C11" s="328" t="s">
+      <c r="B11" s="364"/>
+      <c r="C11" s="327" t="s">
         <v>215</v>
       </c>
-      <c r="D11" s="487"/>
-      <c r="E11" s="487"/>
-      <c r="F11" s="321"/>
-    </row>
-    <row r="12" spans="1:6" s="334" customFormat="1" ht="10.199999999999999">
-      <c r="A12" s="329"/>
-      <c r="B12" s="330" t="s">
+      <c r="D11" s="496"/>
+      <c r="E11" s="508"/>
+      <c r="F11" s="508"/>
+    </row>
+    <row r="12" spans="1:6" s="332" customFormat="1" ht="10.199999999999999">
+      <c r="A12" s="328"/>
+      <c r="B12" s="329" t="s">
         <v>249</v>
       </c>
-      <c r="C12" s="330" t="s">
+      <c r="C12" s="329" t="s">
         <v>291</v>
       </c>
-      <c r="D12" s="355" t="s">
+      <c r="D12" s="352" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="331" t="s">
+      <c r="E12" s="509" t="s">
         <v>297</v>
       </c>
-      <c r="F12" s="333"/>
-    </row>
-    <row r="13" spans="1:6" s="334" customFormat="1" ht="10.199999999999999">
-      <c r="A13" s="329"/>
-      <c r="B13" s="335"/>
-      <c r="C13" s="331"/>
-      <c r="D13" s="370"/>
-      <c r="E13" s="331"/>
-      <c r="F13" s="333"/>
+      <c r="F12" s="509"/>
+    </row>
+    <row r="13" spans="1:6" s="332" customFormat="1" ht="10.199999999999999">
+      <c r="A13" s="328"/>
+      <c r="B13" s="333"/>
+      <c r="C13" s="330"/>
+      <c r="D13" s="365"/>
+      <c r="E13" s="509"/>
+      <c r="F13" s="509"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="322"/>
-      <c r="B14" s="371"/>
-      <c r="C14" s="372"/>
-      <c r="D14" s="338">
+      <c r="B14" s="366"/>
+      <c r="C14" s="367"/>
+      <c r="D14" s="336">
         <f>SUM(D12:D13)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="338">
+      <c r="E14" s="507">
         <f>SUM(E12:E13)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="321"/>
+      <c r="F14" s="507"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="322"/>
@@ -9287,16 +9302,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="322"/>
-      <c r="B16" s="349"/>
-      <c r="C16" s="379" t="s">
+      <c r="B16" s="346"/>
+      <c r="C16" s="374" t="s">
         <v>242</v>
       </c>
-      <c r="D16" s="380"/>
-      <c r="E16" s="344">
+      <c r="D16" s="375"/>
+      <c r="E16" s="341">
         <f>SUM(E12:E13)*42/1000000</f>
         <v>0</v>
       </c>
-      <c r="F16" s="345" t="s">
+      <c r="F16" s="342" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9313,7 +9328,7 @@
       <c r="F19" s="321"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="346" t="s">
+      <c r="A20" s="343" t="s">
         <v>243</v>
       </c>
       <c r="F20" s="321"/>
@@ -9323,13 +9338,13 @@
       <c r="F21" s="321"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="347" t="s">
+      <c r="A22" s="344" t="s">
         <v>244</v>
       </c>
       <c r="F22" s="321"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="347" t="s">
+      <c r="A23" s="344" t="s">
         <v>220</v>
       </c>
       <c r="F23" s="321"/>
@@ -9339,19 +9354,19 @@
       <c r="F24" s="321"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="348" t="s">
+      <c r="A25" s="345" t="s">
         <v>245</v>
       </c>
       <c r="F25" s="321"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="348" t="s">
+      <c r="A26" s="345" t="s">
         <v>246</v>
       </c>
       <c r="F26" s="321"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="348" t="s">
+      <c r="A27" s="345" t="s">
         <v>247</v>
       </c>
       <c r="F27" s="321"/>
@@ -9364,34 +9379,34 @@
       <c r="A29" s="322" t="s">
         <v>224</v>
       </c>
-      <c r="E29" s="373"/>
+      <c r="E29" s="368"/>
       <c r="F29" s="321"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="347" t="s">
+      <c r="A30" s="344" t="s">
         <v>248</v>
       </c>
-      <c r="E30" s="373"/>
+      <c r="E30" s="368"/>
       <c r="F30" s="321"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="347"/>
-      <c r="E31" s="373"/>
+      <c r="A31" s="344"/>
+      <c r="E31" s="368"/>
       <c r="F31" s="321"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="347"/>
-      <c r="E32" s="373"/>
+      <c r="A32" s="344"/>
+      <c r="E32" s="368"/>
       <c r="F32" s="321"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="347"/>
-      <c r="E33" s="373"/>
+      <c r="A33" s="344"/>
+      <c r="E33" s="368"/>
       <c r="F33" s="321"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="347"/>
-      <c r="E34" s="373"/>
+      <c r="A34" s="344"/>
+      <c r="E34" s="368"/>
       <c r="F34" s="321"/>
     </row>
     <row r="35" spans="1:6">
@@ -9399,16 +9414,16 @@
       <c r="F35" s="321"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="508" t="s">
+      <c r="A36" s="376" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="351" t="s">
+      <c r="B36" s="348" t="s">
         <v>226</v>
       </c>
-      <c r="C36" s="352" t="s">
+      <c r="C36" s="349" t="s">
         <v>227</v>
       </c>
-      <c r="D36" s="351" t="s">
+      <c r="D36" s="348" t="s">
         <v>228</v>
       </c>
       <c r="E36" s="501" t="s">
@@ -9417,16 +9432,16 @@
       <c r="F36" s="502"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="509">
+      <c r="A37" s="377">
         <v>0</v>
       </c>
-      <c r="B37" s="354">
+      <c r="B37" s="351">
         <v>41331</v>
       </c>
-      <c r="C37" s="352" t="s">
+      <c r="C37" s="349" t="s">
         <v>230</v>
       </c>
-      <c r="D37" s="351" t="s">
+      <c r="D37" s="348" t="s">
         <v>231</v>
       </c>
       <c r="E37" s="503" t="s">
@@ -9435,19 +9450,24 @@
       <c r="F37" s="504"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="349"/>
+      <c r="B38" s="346"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>